<commit_message>
Fix typo in .gitignore file
</commit_message>
<xml_diff>
--- a/assets/synthesegabriel.xlsx
+++ b/assets/synthesegabriel.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="27628"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="10908"/>
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Gabriel\OneDrive - Ecole IPSSI\IPSSI\Portfolio Final\PortfolioGabriel\assets\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://testipformation-my.sharepoint.com/personal/g_martin_ecole-ipssi_net/Documents/IPSSI/Portfolio Final/assets/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{11A09743-F9E9-41CF-B94B-EEA8224A8669}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="1" documentId="8_{11A09743-F9E9-41CF-B94B-EEA8224A8669}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{053D3003-935E-1546-A47B-AD17D6B28B7C}"/>
   <bookViews>
-    <workbookView showHorizontalScroll="0" showVerticalScroll="0" showSheetTabs="0" xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView showHorizontalScroll="0" showVerticalScroll="0" showSheetTabs="0" xWindow="0" yWindow="3220" windowWidth="29400" windowHeight="16980" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Tableau de synthèse Épreuve E4" sheetId="1" r:id="rId1"/>
@@ -166,13 +166,13 @@
     <t>06/05/24 au 26/05/24</t>
   </si>
   <si>
-    <t>01/11/24 au 15/02/24</t>
-  </si>
-  <si>
     <t>Veilles informatiques</t>
   </si>
   <si>
     <t>X</t>
+  </si>
+  <si>
+    <t>du 01/11/24 au 15/02/24</t>
   </si>
 </sst>
 </file>
@@ -714,15 +714,48 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1"/>
     </xf>
+    <xf numFmtId="14" fontId="4" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="20" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="21" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="22" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="25" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="23" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="24" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -755,39 +788,6 @@
     </xf>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="28" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="20" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="21" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="22" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="25" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="23" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="24" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="14" fontId="4" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -1154,70 +1154,70 @@
   </sheetPr>
   <dimension ref="A1:AQ81"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A15" zoomScale="60" zoomScaleNormal="60" workbookViewId="0">
-      <selection activeCell="L6" sqref="L6"/>
+    <sheetView tabSelected="1" topLeftCell="A7" zoomScale="88" zoomScaleNormal="88" workbookViewId="0">
+      <selection activeCell="C11" sqref="C11"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="10.88671875" defaultRowHeight="13.2" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="10.83203125" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
   <cols>
-    <col min="1" max="1" width="70.44140625" style="1" customWidth="1"/>
-    <col min="2" max="2" width="34.21875" style="1" customWidth="1"/>
+    <col min="1" max="1" width="70.5" style="1" customWidth="1"/>
+    <col min="2" max="2" width="34.1640625" style="1" customWidth="1"/>
     <col min="3" max="8" width="18.6640625" style="1" customWidth="1"/>
-    <col min="9" max="43" width="11.44140625" customWidth="1"/>
-    <col min="44" max="16384" width="10.88671875" style="1"/>
+    <col min="9" max="43" width="11.5" customWidth="1"/>
+    <col min="44" max="16384" width="10.83203125" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:43" ht="39.9" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="24" t="s">
+    <row r="1" spans="1:43" ht="40" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A1" s="25" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="24"/>
-      <c r="C1" s="24"/>
-      <c r="D1" s="24"/>
-      <c r="E1" s="24"/>
-      <c r="F1" s="24"/>
-      <c r="G1" s="24" t="s">
+      <c r="B1" s="25"/>
+      <c r="C1" s="25"/>
+      <c r="D1" s="25"/>
+      <c r="E1" s="25"/>
+      <c r="F1" s="25"/>
+      <c r="G1" s="25" t="s">
         <v>1</v>
       </c>
-      <c r="H1" s="24"/>
-    </row>
-    <row r="2" spans="1:43" ht="41.1" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="24" t="s">
+      <c r="H1" s="25"/>
+    </row>
+    <row r="2" spans="1:43" ht="41" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A2" s="25" t="s">
         <v>2</v>
       </c>
-      <c r="B2" s="24"/>
-      <c r="C2" s="24"/>
-      <c r="D2" s="24"/>
-      <c r="E2" s="24"/>
-      <c r="F2" s="24"/>
-      <c r="G2" s="24"/>
-      <c r="H2" s="24"/>
-    </row>
-    <row r="3" spans="1:43" ht="39.9" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="36" t="s">
+      <c r="B2" s="25"/>
+      <c r="C2" s="25"/>
+      <c r="D2" s="25"/>
+      <c r="E2" s="25"/>
+      <c r="F2" s="25"/>
+      <c r="G2" s="25"/>
+      <c r="H2" s="25"/>
+    </row>
+    <row r="3" spans="1:43" ht="40" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A3" s="26" t="s">
         <v>24</v>
       </c>
-      <c r="B3" s="37"/>
-      <c r="C3" s="37"/>
-      <c r="D3" s="37"/>
-      <c r="E3" s="38"/>
-      <c r="F3" s="42" t="s">
+      <c r="B3" s="27"/>
+      <c r="C3" s="27"/>
+      <c r="D3" s="27"/>
+      <c r="E3" s="28"/>
+      <c r="F3" s="32" t="s">
         <v>3</v>
       </c>
-      <c r="G3" s="37"/>
-      <c r="H3" s="43"/>
+      <c r="G3" s="27"/>
+      <c r="H3" s="33"/>
       <c r="K3" s="1"/>
       <c r="L3" s="1"/>
       <c r="M3" s="1"/>
     </row>
-    <row r="4" spans="1:43" ht="39.9" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A4" s="39" t="s">
+    <row r="4" spans="1:43" ht="40" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A4" s="29" t="s">
         <v>26</v>
       </c>
-      <c r="B4" s="40"/>
-      <c r="C4" s="40"/>
-      <c r="D4" s="40"/>
-      <c r="E4" s="41"/>
+      <c r="B4" s="30"/>
+      <c r="C4" s="30"/>
+      <c r="D4" s="30"/>
+      <c r="E4" s="31"/>
       <c r="F4" s="12" t="s">
         <v>4</v>
       </c>
@@ -1228,23 +1228,23 @@
         <v>6</v>
       </c>
     </row>
-    <row r="5" spans="1:43" ht="39.9" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A5" s="33" t="s">
+    <row r="5" spans="1:43" ht="40" customHeight="1" thickBot="1" x14ac:dyDescent="0.2">
+      <c r="A5" s="44" t="s">
         <v>25</v>
       </c>
-      <c r="B5" s="34"/>
-      <c r="C5" s="34"/>
-      <c r="D5" s="34"/>
-      <c r="E5" s="34"/>
-      <c r="F5" s="34"/>
-      <c r="G5" s="34"/>
-      <c r="H5" s="35"/>
-    </row>
-    <row r="6" spans="1:43" ht="90" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A6" s="22" t="s">
+      <c r="B5" s="45"/>
+      <c r="C5" s="45"/>
+      <c r="D5" s="45"/>
+      <c r="E5" s="45"/>
+      <c r="F5" s="45"/>
+      <c r="G5" s="45"/>
+      <c r="H5" s="46"/>
+    </row>
+    <row r="6" spans="1:43" ht="90" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A6" s="34" t="s">
         <v>7</v>
       </c>
-      <c r="B6" s="31" t="s">
+      <c r="B6" s="42" t="s">
         <v>8</v>
       </c>
       <c r="C6" s="6" t="s">
@@ -1266,9 +1266,9 @@
         <v>14</v>
       </c>
     </row>
-    <row r="7" spans="1:43" s="2" customFormat="1" ht="324.89999999999998" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A7" s="23"/>
-      <c r="B7" s="32"/>
+    <row r="7" spans="1:43" s="2" customFormat="1" ht="325" customHeight="1" thickBot="1" x14ac:dyDescent="0.2">
+      <c r="A7" s="35"/>
+      <c r="B7" s="43"/>
       <c r="C7" s="20" t="s">
         <v>15</v>
       </c>
@@ -1323,17 +1323,17 @@
       <c r="AP7"/>
       <c r="AQ7"/>
     </row>
-    <row r="8" spans="1:43" s="2" customFormat="1" ht="17.399999999999999" x14ac:dyDescent="0.25">
-      <c r="A8" s="25" t="s">
+    <row r="8" spans="1:43" s="2" customFormat="1" ht="18" x14ac:dyDescent="0.15">
+      <c r="A8" s="36" t="s">
         <v>21</v>
       </c>
-      <c r="B8" s="26"/>
-      <c r="C8" s="26"/>
-      <c r="D8" s="26"/>
-      <c r="E8" s="26"/>
-      <c r="F8" s="26"/>
-      <c r="G8" s="26"/>
-      <c r="H8" s="27"/>
+      <c r="B8" s="37"/>
+      <c r="C8" s="37"/>
+      <c r="D8" s="37"/>
+      <c r="E8" s="37"/>
+      <c r="F8" s="37"/>
+      <c r="G8" s="37"/>
+      <c r="H8" s="38"/>
       <c r="I8"/>
       <c r="J8"/>
       <c r="K8"/>
@@ -1370,20 +1370,20 @@
       <c r="AP8"/>
       <c r="AQ8"/>
     </row>
-    <row r="9" spans="1:43" s="2" customFormat="1" ht="39.9" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:43" s="2" customFormat="1" ht="40" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A9" s="9" t="s">
         <v>27</v>
       </c>
       <c r="B9" s="8" t="s">
-        <v>35</v>
+        <v>37</v>
       </c>
       <c r="C9" s="14"/>
       <c r="D9" s="15"/>
       <c r="E9" s="15"/>
       <c r="F9" s="15"/>
       <c r="G9" s="15"/>
-      <c r="H9" s="45" t="s">
-        <v>37</v>
+      <c r="H9" s="23" t="s">
+        <v>36</v>
       </c>
       <c r="I9"/>
       <c r="J9"/>
@@ -1421,7 +1421,7 @@
       <c r="AP9"/>
       <c r="AQ9"/>
     </row>
-    <row r="10" spans="1:43" s="2" customFormat="1" ht="39.9" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:43" s="2" customFormat="1" ht="40" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A10" s="9" t="s">
         <v>28</v>
       </c>
@@ -1431,8 +1431,8 @@
       <c r="E10" s="15"/>
       <c r="F10" s="15"/>
       <c r="G10" s="15"/>
-      <c r="H10" s="45" t="s">
-        <v>37</v>
+      <c r="H10" s="23" t="s">
+        <v>36</v>
       </c>
       <c r="I10"/>
       <c r="J10"/>
@@ -1470,9 +1470,9 @@
       <c r="AP10"/>
       <c r="AQ10"/>
     </row>
-    <row r="11" spans="1:43" s="2" customFormat="1" ht="39.9" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:43" s="2" customFormat="1" ht="40" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A11" s="9" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="B11" s="8"/>
       <c r="C11" s="15"/>
@@ -1480,8 +1480,8 @@
       <c r="E11" s="15"/>
       <c r="F11" s="15"/>
       <c r="G11" s="15"/>
-      <c r="H11" s="45" t="s">
-        <v>37</v>
+      <c r="H11" s="23" t="s">
+        <v>36</v>
       </c>
       <c r="I11"/>
       <c r="J11"/>
@@ -1519,7 +1519,7 @@
       <c r="AP11"/>
       <c r="AQ11"/>
     </row>
-    <row r="12" spans="1:43" s="2" customFormat="1" ht="39.9" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:43" s="2" customFormat="1" ht="40" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A12" s="9"/>
       <c r="B12" s="8"/>
       <c r="C12" s="15"/>
@@ -1564,7 +1564,7 @@
       <c r="AP12"/>
       <c r="AQ12"/>
     </row>
-    <row r="13" spans="1:43" s="2" customFormat="1" ht="39.9" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:43" s="2" customFormat="1" ht="40" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A13" s="9"/>
       <c r="B13" s="8"/>
       <c r="C13" s="15"/>
@@ -1609,7 +1609,7 @@
       <c r="AP13"/>
       <c r="AQ13"/>
     </row>
-    <row r="14" spans="1:43" s="2" customFormat="1" ht="39.9" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:43" s="2" customFormat="1" ht="40" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A14" s="9"/>
       <c r="B14" s="8"/>
       <c r="C14" s="15"/>
@@ -1654,7 +1654,7 @@
       <c r="AP14"/>
       <c r="AQ14"/>
     </row>
-    <row r="15" spans="1:43" s="2" customFormat="1" ht="39.9" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:43" s="2" customFormat="1" ht="40" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A15" s="9"/>
       <c r="B15" s="8"/>
       <c r="C15" s="15"/>
@@ -1699,7 +1699,7 @@
       <c r="AP15"/>
       <c r="AQ15"/>
     </row>
-    <row r="16" spans="1:43" s="2" customFormat="1" ht="39.9" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:43" s="2" customFormat="1" ht="40" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A16" s="9"/>
       <c r="B16" s="8"/>
       <c r="C16" s="15"/>
@@ -1744,7 +1744,7 @@
       <c r="AP16"/>
       <c r="AQ16"/>
     </row>
-    <row r="17" spans="1:43" s="2" customFormat="1" ht="39.9" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:43" s="2" customFormat="1" ht="40" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A17" s="9"/>
       <c r="B17" s="8"/>
       <c r="C17" s="15"/>
@@ -1789,7 +1789,7 @@
       <c r="AP17"/>
       <c r="AQ17"/>
     </row>
-    <row r="18" spans="1:43" s="2" customFormat="1" ht="39.9" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:43" s="2" customFormat="1" ht="40" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A18" s="9"/>
       <c r="B18" s="8"/>
       <c r="C18" s="15"/>
@@ -1834,17 +1834,17 @@
       <c r="AP18"/>
       <c r="AQ18"/>
     </row>
-    <row r="19" spans="1:43" s="2" customFormat="1" ht="17.399999999999999" x14ac:dyDescent="0.25">
-      <c r="A19" s="28" t="s">
+    <row r="19" spans="1:43" s="2" customFormat="1" ht="18" x14ac:dyDescent="0.15">
+      <c r="A19" s="39" t="s">
         <v>22</v>
       </c>
-      <c r="B19" s="29"/>
-      <c r="C19" s="29"/>
-      <c r="D19" s="29"/>
-      <c r="E19" s="29"/>
-      <c r="F19" s="29"/>
-      <c r="G19" s="29"/>
-      <c r="H19" s="30"/>
+      <c r="B19" s="40"/>
+      <c r="C19" s="40"/>
+      <c r="D19" s="40"/>
+      <c r="E19" s="40"/>
+      <c r="F19" s="40"/>
+      <c r="G19" s="40"/>
+      <c r="H19" s="41"/>
       <c r="I19"/>
       <c r="J19"/>
       <c r="K19"/>
@@ -1881,19 +1881,19 @@
       <c r="AP19"/>
       <c r="AQ19"/>
     </row>
-    <row r="20" spans="1:43" s="2" customFormat="1" ht="39.9" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:43" s="2" customFormat="1" ht="40" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A20" s="9" t="s">
         <v>29</v>
       </c>
-      <c r="B20" s="44" t="s">
+      <c r="B20" s="22" t="s">
         <v>32</v>
       </c>
       <c r="C20" s="15"/>
       <c r="D20" s="15"/>
       <c r="E20" s="15"/>
       <c r="F20" s="15"/>
-      <c r="G20" s="46" t="s">
-        <v>37</v>
+      <c r="G20" s="24" t="s">
+        <v>36</v>
       </c>
       <c r="H20" s="16"/>
       <c r="I20"/>
@@ -1932,7 +1932,7 @@
       <c r="AP20"/>
       <c r="AQ20"/>
     </row>
-    <row r="21" spans="1:43" s="2" customFormat="1" ht="39.9" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:43" s="2" customFormat="1" ht="40" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A21" s="9" t="s">
         <v>30</v>
       </c>
@@ -1943,8 +1943,8 @@
       <c r="D21" s="15"/>
       <c r="E21" s="15"/>
       <c r="F21" s="15"/>
-      <c r="G21" s="46" t="s">
-        <v>37</v>
+      <c r="G21" s="24" t="s">
+        <v>36</v>
       </c>
       <c r="H21" s="16"/>
       <c r="I21"/>
@@ -1983,7 +1983,7 @@
       <c r="AP21"/>
       <c r="AQ21"/>
     </row>
-    <row r="22" spans="1:43" s="2" customFormat="1" ht="39.9" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:43" s="2" customFormat="1" ht="40" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A22" s="9" t="s">
         <v>31</v>
       </c>
@@ -1992,8 +1992,8 @@
       </c>
       <c r="C22" s="15"/>
       <c r="D22" s="15"/>
-      <c r="E22" s="46" t="s">
-        <v>37</v>
+      <c r="E22" s="24" t="s">
+        <v>36</v>
       </c>
       <c r="F22" s="15"/>
       <c r="G22" s="15"/>
@@ -2034,7 +2034,7 @@
       <c r="AP22"/>
       <c r="AQ22"/>
     </row>
-    <row r="23" spans="1:43" s="2" customFormat="1" ht="39.9" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:43" s="2" customFormat="1" ht="40" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A23" s="9"/>
       <c r="B23" s="8"/>
       <c r="C23" s="15"/>
@@ -2079,7 +2079,7 @@
       <c r="AP23"/>
       <c r="AQ23"/>
     </row>
-    <row r="24" spans="1:43" s="2" customFormat="1" ht="39.9" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:43" s="2" customFormat="1" ht="40" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A24" s="9"/>
       <c r="B24" s="8"/>
       <c r="C24" s="15"/>
@@ -2124,7 +2124,7 @@
       <c r="AP24"/>
       <c r="AQ24"/>
     </row>
-    <row r="25" spans="1:43" s="2" customFormat="1" ht="39.9" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:43" s="2" customFormat="1" ht="40" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A25" s="9"/>
       <c r="B25" s="8"/>
       <c r="C25" s="15"/>
@@ -2169,7 +2169,7 @@
       <c r="AP25"/>
       <c r="AQ25"/>
     </row>
-    <row r="26" spans="1:43" s="2" customFormat="1" ht="39.9" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:43" s="2" customFormat="1" ht="40" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A26" s="9"/>
       <c r="B26" s="8"/>
       <c r="C26" s="15"/>
@@ -2214,17 +2214,17 @@
       <c r="AP26"/>
       <c r="AQ26"/>
     </row>
-    <row r="27" spans="1:43" s="2" customFormat="1" ht="17.399999999999999" x14ac:dyDescent="0.25">
-      <c r="A27" s="28" t="s">
+    <row r="27" spans="1:43" s="2" customFormat="1" ht="18" x14ac:dyDescent="0.15">
+      <c r="A27" s="39" t="s">
         <v>23</v>
       </c>
-      <c r="B27" s="29"/>
-      <c r="C27" s="29"/>
-      <c r="D27" s="29"/>
-      <c r="E27" s="29"/>
-      <c r="F27" s="29"/>
-      <c r="G27" s="29"/>
-      <c r="H27" s="30"/>
+      <c r="B27" s="40"/>
+      <c r="C27" s="40"/>
+      <c r="D27" s="40"/>
+      <c r="E27" s="40"/>
+      <c r="F27" s="40"/>
+      <c r="G27" s="40"/>
+      <c r="H27" s="41"/>
       <c r="I27"/>
       <c r="J27"/>
       <c r="K27"/>
@@ -2261,7 +2261,7 @@
       <c r="AP27"/>
       <c r="AQ27"/>
     </row>
-    <row r="28" spans="1:43" s="2" customFormat="1" ht="39.9" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:43" s="2" customFormat="1" ht="40" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A28" s="9"/>
       <c r="B28" s="8"/>
       <c r="C28" s="15"/>
@@ -2306,7 +2306,7 @@
       <c r="AP28"/>
       <c r="AQ28"/>
     </row>
-    <row r="29" spans="1:43" s="2" customFormat="1" ht="39.9" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:43" s="2" customFormat="1" ht="40" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A29" s="9"/>
       <c r="B29" s="8"/>
       <c r="C29" s="15"/>
@@ -2351,7 +2351,7 @@
       <c r="AP29"/>
       <c r="AQ29"/>
     </row>
-    <row r="30" spans="1:43" s="2" customFormat="1" ht="39.9" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:43" s="2" customFormat="1" ht="40" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A30" s="9"/>
       <c r="B30" s="8"/>
       <c r="C30" s="15"/>
@@ -2396,7 +2396,7 @@
       <c r="AP30"/>
       <c r="AQ30"/>
     </row>
-    <row r="31" spans="1:43" s="2" customFormat="1" ht="39.9" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:43" s="2" customFormat="1" ht="40" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A31" s="9"/>
       <c r="B31" s="8"/>
       <c r="C31" s="15"/>
@@ -2441,7 +2441,7 @@
       <c r="AP31"/>
       <c r="AQ31"/>
     </row>
-    <row r="32" spans="1:43" s="2" customFormat="1" ht="39.9" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:43" s="2" customFormat="1" ht="40" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A32" s="9"/>
       <c r="B32" s="8"/>
       <c r="C32" s="15"/>
@@ -2486,7 +2486,7 @@
       <c r="AP32"/>
       <c r="AQ32"/>
     </row>
-    <row r="33" spans="1:43" s="2" customFormat="1" ht="39.9" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:43" s="2" customFormat="1" ht="40" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A33" s="9"/>
       <c r="B33" s="8"/>
       <c r="C33" s="15"/>
@@ -2531,7 +2531,7 @@
       <c r="AP33"/>
       <c r="AQ33"/>
     </row>
-    <row r="34" spans="1:43" s="2" customFormat="1" ht="39.9" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="34" spans="1:43" s="2" customFormat="1" ht="40" customHeight="1" thickBot="1" x14ac:dyDescent="0.2">
       <c r="A34" s="10"/>
       <c r="B34" s="11"/>
       <c r="C34" s="17"/>
@@ -2576,7 +2576,7 @@
       <c r="AP34"/>
       <c r="AQ34"/>
     </row>
-    <row r="35" spans="1:43" s="2" customFormat="1" ht="13.8" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:43" s="2" customFormat="1" ht="14" x14ac:dyDescent="0.15">
       <c r="A35" s="5"/>
       <c r="B35" s="3"/>
       <c r="C35" s="4"/>
@@ -2621,59 +2621,54 @@
       <c r="AP35"/>
       <c r="AQ35"/>
     </row>
-    <row r="36" spans="1:43" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="37" spans="1:43" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="38" spans="1:43" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="39" spans="1:43" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="40" spans="1:43" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="41" spans="1:43" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="42" spans="1:43" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="43" spans="1:43" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="44" spans="1:43" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="45" spans="1:43" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="46" spans="1:43" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="47" spans="1:43" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="48" spans="1:43" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="49" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="50" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="51" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="52" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="53" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="54" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="55" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="56" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="57" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="58" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="59" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="60" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="61" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="62" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="63" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="64" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="65" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="66" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="67" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="68" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="69" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="70" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="71" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="72" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="73" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="74" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="75" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="76" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="77" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="78" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="79" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="80" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="81" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="36" spans="1:43" customFormat="1" x14ac:dyDescent="0.15"/>
+    <row r="37" spans="1:43" customFormat="1" x14ac:dyDescent="0.15"/>
+    <row r="38" spans="1:43" customFormat="1" x14ac:dyDescent="0.15"/>
+    <row r="39" spans="1:43" customFormat="1" x14ac:dyDescent="0.15"/>
+    <row r="40" spans="1:43" customFormat="1" x14ac:dyDescent="0.15"/>
+    <row r="41" spans="1:43" customFormat="1" x14ac:dyDescent="0.15"/>
+    <row r="42" spans="1:43" customFormat="1" x14ac:dyDescent="0.15"/>
+    <row r="43" spans="1:43" customFormat="1" x14ac:dyDescent="0.15"/>
+    <row r="44" spans="1:43" customFormat="1" x14ac:dyDescent="0.15"/>
+    <row r="45" spans="1:43" customFormat="1" x14ac:dyDescent="0.15"/>
+    <row r="46" spans="1:43" customFormat="1" x14ac:dyDescent="0.15"/>
+    <row r="47" spans="1:43" customFormat="1" x14ac:dyDescent="0.15"/>
+    <row r="48" spans="1:43" customFormat="1" x14ac:dyDescent="0.15"/>
+    <row r="49" customFormat="1" x14ac:dyDescent="0.15"/>
+    <row r="50" customFormat="1" x14ac:dyDescent="0.15"/>
+    <row r="51" customFormat="1" x14ac:dyDescent="0.15"/>
+    <row r="52" customFormat="1" x14ac:dyDescent="0.15"/>
+    <row r="53" customFormat="1" x14ac:dyDescent="0.15"/>
+    <row r="54" customFormat="1" x14ac:dyDescent="0.15"/>
+    <row r="55" customFormat="1" x14ac:dyDescent="0.15"/>
+    <row r="56" customFormat="1" x14ac:dyDescent="0.15"/>
+    <row r="57" customFormat="1" x14ac:dyDescent="0.15"/>
+    <row r="58" customFormat="1" x14ac:dyDescent="0.15"/>
+    <row r="59" customFormat="1" x14ac:dyDescent="0.15"/>
+    <row r="60" customFormat="1" x14ac:dyDescent="0.15"/>
+    <row r="61" customFormat="1" x14ac:dyDescent="0.15"/>
+    <row r="62" customFormat="1" x14ac:dyDescent="0.15"/>
+    <row r="63" customFormat="1" x14ac:dyDescent="0.15"/>
+    <row r="64" customFormat="1" x14ac:dyDescent="0.15"/>
+    <row r="65" customFormat="1" x14ac:dyDescent="0.15"/>
+    <row r="66" customFormat="1" x14ac:dyDescent="0.15"/>
+    <row r="67" customFormat="1" x14ac:dyDescent="0.15"/>
+    <row r="68" customFormat="1" x14ac:dyDescent="0.15"/>
+    <row r="69" customFormat="1" x14ac:dyDescent="0.15"/>
+    <row r="70" customFormat="1" x14ac:dyDescent="0.15"/>
+    <row r="71" customFormat="1" x14ac:dyDescent="0.15"/>
+    <row r="72" customFormat="1" x14ac:dyDescent="0.15"/>
+    <row r="73" customFormat="1" x14ac:dyDescent="0.15"/>
+    <row r="74" customFormat="1" x14ac:dyDescent="0.15"/>
+    <row r="75" customFormat="1" x14ac:dyDescent="0.15"/>
+    <row r="76" customFormat="1" x14ac:dyDescent="0.15"/>
+    <row r="77" customFormat="1" x14ac:dyDescent="0.15"/>
+    <row r="78" customFormat="1" x14ac:dyDescent="0.15"/>
+    <row r="79" customFormat="1" x14ac:dyDescent="0.15"/>
+    <row r="80" customFormat="1" x14ac:dyDescent="0.15"/>
+    <row r="81" customFormat="1" x14ac:dyDescent="0.15"/>
   </sheetData>
   <mergeCells count="12">
-    <mergeCell ref="G1:H1"/>
-    <mergeCell ref="A1:F1"/>
-    <mergeCell ref="A3:E3"/>
-    <mergeCell ref="A4:E4"/>
-    <mergeCell ref="F3:H3"/>
     <mergeCell ref="A6:A7"/>
     <mergeCell ref="A2:H2"/>
     <mergeCell ref="A8:H8"/>
@@ -2681,6 +2676,11 @@
     <mergeCell ref="A27:H27"/>
     <mergeCell ref="B6:B7"/>
     <mergeCell ref="A5:H5"/>
+    <mergeCell ref="G1:H1"/>
+    <mergeCell ref="A1:F1"/>
+    <mergeCell ref="A3:E3"/>
+    <mergeCell ref="A4:E4"/>
+    <mergeCell ref="F3:H3"/>
   </mergeCells>
   <phoneticPr fontId="2" type="noConversion"/>
   <printOptions horizontalCentered="1" verticalCentered="1"/>
@@ -2692,17 +2692,6 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement>
-    <lcf76f155ced4ddcb4097134ff3c332f xmlns="44fce352-7b49-42d3-bc69-12da48d9ebc0">
-      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    </lcf76f155ced4ddcb4097134ff3c332f>
-    <TaxCatchAll xmlns="fbb90945-3c4c-43b7-bb15-9ae99079c100" xsi:nil="true"/>
-  </documentManagement>
-</p:properties>
-</file>
-
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x010100B44D25FE6749554FA89155DE40CE9E1E" ma:contentTypeVersion="14" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="8bb8039247b655a9c70bf36b5dd9dc64">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="44fce352-7b49-42d3-bc69-12da48d9ebc0" xmlns:ns3="fbb90945-3c4c-43b7-bb15-9ae99079c100" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="85d91c69c6e00024127dca24cda9fdf4" ns2:_="" ns3:_="">
     <xsd:import namespace="44fce352-7b49-42d3-bc69-12da48d9ebc0"/>
@@ -2931,6 +2920,17 @@
 </ct:contentTypeSchema>
 </file>
 
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement>
+    <lcf76f155ced4ddcb4097134ff3c332f xmlns="44fce352-7b49-42d3-bc69-12da48d9ebc0">
+      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    </lcf76f155ced4ddcb4097134ff3c332f>
+    <TaxCatchAll xmlns="fbb90945-3c4c-43b7-bb15-9ae99079c100" xsi:nil="true"/>
+  </documentManagement>
+</p:properties>
+</file>
+
 <file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <?mso-contentType ?>
 <FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
@@ -2941,17 +2941,6 @@
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{CD1FC233-9ECF-4A55-86D4-136E16072842}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="44fce352-7b49-42d3-bc69-12da48d9ebc0"/>
-    <ds:schemaRef ds:uri="fbb90945-3c4c-43b7-bb15-9ae99079c100"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{36ECBC65-C27A-4C6D-BAE3-04A998F6FAE4}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -2970,6 +2959,23 @@
 </ds:datastoreItem>
 </file>
 
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{CD1FC233-9ECF-4A55-86D4-136E16072842}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="fbb90945-3c4c-43b7-bb15-9ae99079c100"/>
+    <ds:schemaRef ds:uri="44fce352-7b49-42d3-bc69-12da48d9ebc0"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
 <file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{4209C33D-ED08-404F-9B7A-29CD40C2ACA2}">
   <ds:schemaRefs>

</xml_diff>

<commit_message>
Add documentation section and improve content in index.html; update styles in style.css
</commit_message>
<xml_diff>
--- a/assets/synthesegabriel.xlsx
+++ b/assets/synthesegabriel.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="10908"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="11013"/>
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://testipformation-my.sharepoint.com/personal/g_martin_ecole-ipssi_net/Documents/IPSSI/Portfolio Final/assets/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="1" documentId="8_{11A09743-F9E9-41CF-B94B-EEA8224A8669}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{053D3003-935E-1546-A47B-AD17D6B28B7C}"/>
+  <xr:revisionPtr revIDLastSave="69" documentId="8_{11A09743-F9E9-41CF-B94B-EEA8224A8669}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{2BAE55F8-ADA7-4545-BF49-70902B85047C}"/>
   <bookViews>
-    <workbookView showHorizontalScroll="0" showVerticalScroll="0" showSheetTabs="0" xWindow="0" yWindow="3220" windowWidth="29400" windowHeight="16980" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView showHorizontalScroll="0" showVerticalScroll="0" showSheetTabs="0" xWindow="0" yWindow="900" windowWidth="29400" windowHeight="16980" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Tableau de synthèse Épreuve E4" sheetId="1" r:id="rId1"/>
@@ -39,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="43" uniqueCount="38">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="61" uniqueCount="48">
   <si>
     <t>BTS SERVICES INFORMATIQUES AUX ORGANISATIONS</t>
   </si>
@@ -141,38 +141,70 @@
     <t>Centre de formation : Ecole IPSSI</t>
   </si>
   <si>
-    <t xml:space="preserve">Projet AP1 </t>
-  </si>
-  <si>
-    <t xml:space="preserve">Réalisation de mon portfolio
+    <t>Installation d'une VM Ubuntu</t>
+  </si>
+  <si>
+    <t>Connexion WSL entre VSCode et la VM</t>
+  </si>
+  <si>
+    <t>Maintenance d'une application web</t>
+  </si>
+  <si>
+    <t>17/06/2024 au 19/06/24</t>
+  </si>
+  <si>
+    <t>19/06/24 au 22/06/24</t>
+  </si>
+  <si>
+    <t>06/05/24 au 26/05/24</t>
+  </si>
+  <si>
+    <t>Veilles informatiques</t>
+  </si>
+  <si>
+    <t>X</t>
+  </si>
+  <si>
+    <t>du 01/11/24 au 15/02/24</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Inventaire matériel réseau
 </t>
   </si>
   <si>
-    <t>Installation d'une VM Ubuntu</t>
-  </si>
-  <si>
-    <t>Connexion WSL entre VSCode et la VM</t>
-  </si>
-  <si>
-    <t>Maintenance d'une application web</t>
-  </si>
-  <si>
-    <t>17/06/2024 au 19/06/24</t>
-  </si>
-  <si>
-    <t>19/06/24 au 22/06/24</t>
-  </si>
-  <si>
-    <t>06/05/24 au 26/05/24</t>
-  </si>
-  <si>
-    <t>Veilles informatiques</t>
-  </si>
-  <si>
-    <t>X</t>
-  </si>
-  <si>
-    <t>du 01/11/24 au 15/02/24</t>
+    <t>Documentation GLPI</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Réalisation de mon Portfolio
+</t>
+  </si>
+  <si>
+    <t>Réalisation du site web InfoLab</t>
+  </si>
+  <si>
+    <t>Documentation + Réalisation du site web GSB</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Documentation + Réalisation de l'application GSB
+</t>
+  </si>
+  <si>
+    <t>le 16/09/2024</t>
+  </si>
+  <si>
+    <t>du 10/01/2023 au 05/06/2025</t>
+  </si>
+  <si>
+    <t>le 30/09/2024</t>
+  </si>
+  <si>
+    <t>du 16/09/2024 au 23/05/2024</t>
+  </si>
+  <si>
+    <t>du 08/01/2024 au 23/05/2024</t>
+  </si>
+  <si>
+    <t>du 10/04/2023 au 23/05/2024</t>
   </si>
 </sst>
 </file>
@@ -649,7 +681,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="164" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="47">
+  <cellXfs count="49">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="center"/>
@@ -788,6 +820,12 @@
     </xf>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="28" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -860,6 +898,10 @@
     <xdr:clientData/>
   </xdr:twoCellAnchor>
 </xdr:wsDr>
+</file>
+
+<file path=xl/persons/person.xml><?xml version="1.0" encoding="utf-8"?>
+<personList xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main"/>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -1154,8 +1196,8 @@
   </sheetPr>
   <dimension ref="A1:AQ81"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A7" zoomScale="88" zoomScaleNormal="88" workbookViewId="0">
-      <selection activeCell="C11" sqref="C11"/>
+    <sheetView tabSelected="1" topLeftCell="A22" zoomScale="88" zoomScaleNormal="88" workbookViewId="0">
+      <selection activeCell="B16" sqref="B16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="10.83203125" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
@@ -1372,19 +1414,19 @@
     </row>
     <row r="9" spans="1:43" s="2" customFormat="1" ht="40" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A9" s="9" t="s">
-        <v>27</v>
+        <v>39</v>
       </c>
       <c r="B9" s="8" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
       <c r="C9" s="14"/>
-      <c r="D9" s="15"/>
-      <c r="E9" s="15"/>
+      <c r="D9" s="24" t="s">
+        <v>34</v>
+      </c>
+      <c r="E9" s="48"/>
       <c r="F9" s="15"/>
       <c r="G9" s="15"/>
-      <c r="H9" s="23" t="s">
-        <v>36</v>
-      </c>
+      <c r="H9" s="23"/>
       <c r="I9"/>
       <c r="J9"/>
       <c r="K9"/>
@@ -1423,17 +1465,19 @@
     </row>
     <row r="10" spans="1:43" s="2" customFormat="1" ht="40" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A10" s="9" t="s">
-        <v>28</v>
-      </c>
-      <c r="B10" s="8"/>
-      <c r="C10" s="15"/>
+        <v>36</v>
+      </c>
+      <c r="B10" s="8" t="s">
+        <v>42</v>
+      </c>
+      <c r="C10" s="24" t="s">
+        <v>34</v>
+      </c>
       <c r="D10" s="15"/>
       <c r="E10" s="15"/>
       <c r="F10" s="15"/>
       <c r="G10" s="15"/>
-      <c r="H10" s="23" t="s">
-        <v>36</v>
-      </c>
+      <c r="H10" s="23"/>
       <c r="I10"/>
       <c r="J10"/>
       <c r="K10"/>
@@ -1472,16 +1516,18 @@
     </row>
     <row r="11" spans="1:43" s="2" customFormat="1" ht="40" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A11" s="9" t="s">
-        <v>35</v>
-      </c>
-      <c r="B11" s="8"/>
+        <v>33</v>
+      </c>
+      <c r="B11" s="8" t="s">
+        <v>43</v>
+      </c>
       <c r="C11" s="15"/>
       <c r="D11" s="15"/>
       <c r="E11" s="15"/>
       <c r="F11" s="15"/>
       <c r="G11" s="15"/>
       <c r="H11" s="23" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
       <c r="I11"/>
       <c r="J11"/>
@@ -1520,13 +1566,23 @@
       <c r="AQ11"/>
     </row>
     <row r="12" spans="1:43" s="2" customFormat="1" ht="40" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A12" s="9"/>
-      <c r="B12" s="8"/>
-      <c r="C12" s="15"/>
-      <c r="D12" s="15"/>
+      <c r="A12" s="9" t="s">
+        <v>37</v>
+      </c>
+      <c r="B12" s="8" t="s">
+        <v>44</v>
+      </c>
+      <c r="C12" s="24" t="s">
+        <v>34</v>
+      </c>
+      <c r="D12" s="24" t="s">
+        <v>34</v>
+      </c>
       <c r="E12" s="15"/>
-      <c r="F12" s="15"/>
-      <c r="G12" s="15"/>
+      <c r="F12" s="24"/>
+      <c r="G12" s="24" t="s">
+        <v>34</v>
+      </c>
       <c r="H12" s="16"/>
       <c r="I12"/>
       <c r="J12"/>
@@ -1565,14 +1621,22 @@
       <c r="AQ12"/>
     </row>
     <row r="13" spans="1:43" s="2" customFormat="1" ht="40" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A13" s="9"/>
-      <c r="B13" s="8"/>
+      <c r="A13" s="9" t="s">
+        <v>40</v>
+      </c>
+      <c r="B13" s="8" t="s">
+        <v>45</v>
+      </c>
       <c r="C13" s="15"/>
       <c r="D13" s="15"/>
       <c r="E13" s="15"/>
-      <c r="F13" s="15"/>
-      <c r="G13" s="15"/>
-      <c r="H13" s="16"/>
+      <c r="F13" s="24" t="s">
+        <v>34</v>
+      </c>
+      <c r="G13" s="47" t="s">
+        <v>34</v>
+      </c>
+      <c r="H13" s="23"/>
       <c r="I13"/>
       <c r="J13"/>
       <c r="K13"/>
@@ -1610,14 +1674,24 @@
       <c r="AQ13"/>
     </row>
     <row r="14" spans="1:43" s="2" customFormat="1" ht="40" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A14" s="9"/>
-      <c r="B14" s="8"/>
+      <c r="A14" s="9" t="s">
+        <v>41</v>
+      </c>
+      <c r="B14" s="8" t="s">
+        <v>46</v>
+      </c>
       <c r="C14" s="15"/>
       <c r="D14" s="15"/>
       <c r="E14" s="15"/>
-      <c r="F14" s="15"/>
-      <c r="G14" s="15"/>
-      <c r="H14" s="16"/>
+      <c r="F14" s="24" t="s">
+        <v>34</v>
+      </c>
+      <c r="G14" s="24" t="s">
+        <v>34</v>
+      </c>
+      <c r="H14" s="23" t="s">
+        <v>34</v>
+      </c>
       <c r="I14"/>
       <c r="J14"/>
       <c r="K14"/>
@@ -1655,8 +1729,12 @@
       <c r="AQ14"/>
     </row>
     <row r="15" spans="1:43" s="2" customFormat="1" ht="40" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A15" s="9"/>
-      <c r="B15" s="8"/>
+      <c r="A15" s="9" t="s">
+        <v>38</v>
+      </c>
+      <c r="B15" s="8" t="s">
+        <v>47</v>
+      </c>
       <c r="C15" s="15"/>
       <c r="D15" s="15"/>
       <c r="E15" s="15"/>
@@ -1883,17 +1961,17 @@
     </row>
     <row r="20" spans="1:43" s="2" customFormat="1" ht="40" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A20" s="9" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="B20" s="22" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
       <c r="C20" s="15"/>
       <c r="D20" s="15"/>
       <c r="E20" s="15"/>
       <c r="F20" s="15"/>
       <c r="G20" s="24" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
       <c r="H20" s="16"/>
       <c r="I20"/>
@@ -1934,17 +2012,17 @@
     </row>
     <row r="21" spans="1:43" s="2" customFormat="1" ht="40" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A21" s="9" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="B21" s="8" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
       <c r="C21" s="15"/>
       <c r="D21" s="15"/>
       <c r="E21" s="15"/>
       <c r="F21" s="15"/>
       <c r="G21" s="24" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
       <c r="H21" s="16"/>
       <c r="I21"/>
@@ -1985,15 +2063,15 @@
     </row>
     <row r="22" spans="1:43" s="2" customFormat="1" ht="40" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A22" s="9" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="B22" s="8" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="C22" s="15"/>
       <c r="D22" s="15"/>
       <c r="E22" s="24" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
       <c r="F22" s="15"/>
       <c r="G22" s="15"/>
@@ -2962,16 +3040,16 @@
 <file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{CD1FC233-9ECF-4A55-86D4-136E16072842}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
-    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
     <ds:schemaRef ds:uri="fbb90945-3c4c-43b7-bb15-9ae99079c100"/>
     <ds:schemaRef ds:uri="44fce352-7b49-42d3-bc69-12da48d9ebc0"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
     <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>

</xml_diff>

<commit_message>
Update status message for Atelier Pédagogique in index.html
</commit_message>
<xml_diff>
--- a/assets/synthesegabriel.xlsx
+++ b/assets/synthesegabriel.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://testipformation-my.sharepoint.com/personal/g_martin_ecole-ipssi_net/Documents/IPSSI/Portfolio Final/assets/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="69" documentId="8_{11A09743-F9E9-41CF-B94B-EEA8224A8669}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{2BAE55F8-ADA7-4545-BF49-70902B85047C}"/>
+  <xr:revisionPtr revIDLastSave="70" documentId="8_{11A09743-F9E9-41CF-B94B-EEA8224A8669}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{01E1C613-6F9C-274E-816B-4FD364ECBD60}"/>
   <bookViews>
-    <workbookView showHorizontalScroll="0" showVerticalScroll="0" showSheetTabs="0" xWindow="0" yWindow="900" windowWidth="29400" windowHeight="16980" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView showHorizontalScroll="0" showVerticalScroll="0" showSheetTabs="0" xWindow="-20" yWindow="900" windowWidth="29400" windowHeight="16980" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Tableau de synthèse Épreuve E4" sheetId="1" r:id="rId1"/>
@@ -39,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="61" uniqueCount="48">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="62" uniqueCount="49">
   <si>
     <t>BTS SERVICES INFORMATIQUES AUX ORGANISATIONS</t>
   </si>
@@ -205,6 +205,9 @@
   </si>
   <si>
     <t>du 10/04/2023 au 23/05/2024</t>
+  </si>
+  <si>
+    <t>Création de de composant web</t>
   </si>
 </sst>
 </file>
@@ -755,9 +758,54 @@
     <xf numFmtId="0" fontId="11" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="27" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="19" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="28" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="20" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
@@ -781,51 +829,6 @@
     </xf>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="24" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="27" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="19" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="28" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -1196,8 +1199,8 @@
   </sheetPr>
   <dimension ref="A1:AQ81"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A22" zoomScale="88" zoomScaleNormal="88" workbookViewId="0">
-      <selection activeCell="B16" sqref="B16"/>
+    <sheetView tabSelected="1" topLeftCell="A12" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
+      <selection activeCell="B28" sqref="B28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="10.83203125" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
@@ -1210,56 +1213,56 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:43" ht="40" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A1" s="25" t="s">
+      <c r="A1" s="29" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="25"/>
-      <c r="C1" s="25"/>
-      <c r="D1" s="25"/>
-      <c r="E1" s="25"/>
-      <c r="F1" s="25"/>
-      <c r="G1" s="25" t="s">
+      <c r="B1" s="29"/>
+      <c r="C1" s="29"/>
+      <c r="D1" s="29"/>
+      <c r="E1" s="29"/>
+      <c r="F1" s="29"/>
+      <c r="G1" s="29" t="s">
         <v>1</v>
       </c>
-      <c r="H1" s="25"/>
+      <c r="H1" s="29"/>
     </row>
     <row r="2" spans="1:43" ht="41" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A2" s="25" t="s">
+      <c r="A2" s="29" t="s">
         <v>2</v>
       </c>
-      <c r="B2" s="25"/>
-      <c r="C2" s="25"/>
-      <c r="D2" s="25"/>
-      <c r="E2" s="25"/>
-      <c r="F2" s="25"/>
-      <c r="G2" s="25"/>
-      <c r="H2" s="25"/>
+      <c r="B2" s="29"/>
+      <c r="C2" s="29"/>
+      <c r="D2" s="29"/>
+      <c r="E2" s="29"/>
+      <c r="F2" s="29"/>
+      <c r="G2" s="29"/>
+      <c r="H2" s="29"/>
     </row>
     <row r="3" spans="1:43" ht="40" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A3" s="26" t="s">
+      <c r="A3" s="41" t="s">
         <v>24</v>
       </c>
-      <c r="B3" s="27"/>
-      <c r="C3" s="27"/>
-      <c r="D3" s="27"/>
-      <c r="E3" s="28"/>
-      <c r="F3" s="32" t="s">
+      <c r="B3" s="42"/>
+      <c r="C3" s="42"/>
+      <c r="D3" s="42"/>
+      <c r="E3" s="43"/>
+      <c r="F3" s="47" t="s">
         <v>3</v>
       </c>
-      <c r="G3" s="27"/>
-      <c r="H3" s="33"/>
+      <c r="G3" s="42"/>
+      <c r="H3" s="48"/>
       <c r="K3" s="1"/>
       <c r="L3" s="1"/>
       <c r="M3" s="1"/>
     </row>
     <row r="4" spans="1:43" ht="40" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A4" s="29" t="s">
+      <c r="A4" s="44" t="s">
         <v>26</v>
       </c>
-      <c r="B4" s="30"/>
-      <c r="C4" s="30"/>
-      <c r="D4" s="30"/>
-      <c r="E4" s="31"/>
+      <c r="B4" s="45"/>
+      <c r="C4" s="45"/>
+      <c r="D4" s="45"/>
+      <c r="E4" s="46"/>
       <c r="F4" s="12" t="s">
         <v>4</v>
       </c>
@@ -1271,22 +1274,22 @@
       </c>
     </row>
     <row r="5" spans="1:43" ht="40" customHeight="1" thickBot="1" x14ac:dyDescent="0.2">
-      <c r="A5" s="44" t="s">
+      <c r="A5" s="38" t="s">
         <v>25</v>
       </c>
-      <c r="B5" s="45"/>
-      <c r="C5" s="45"/>
-      <c r="D5" s="45"/>
-      <c r="E5" s="45"/>
-      <c r="F5" s="45"/>
-      <c r="G5" s="45"/>
-      <c r="H5" s="46"/>
+      <c r="B5" s="39"/>
+      <c r="C5" s="39"/>
+      <c r="D5" s="39"/>
+      <c r="E5" s="39"/>
+      <c r="F5" s="39"/>
+      <c r="G5" s="39"/>
+      <c r="H5" s="40"/>
     </row>
     <row r="6" spans="1:43" ht="90" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A6" s="34" t="s">
+      <c r="A6" s="27" t="s">
         <v>7</v>
       </c>
-      <c r="B6" s="42" t="s">
+      <c r="B6" s="36" t="s">
         <v>8</v>
       </c>
       <c r="C6" s="6" t="s">
@@ -1309,8 +1312,8 @@
       </c>
     </row>
     <row r="7" spans="1:43" s="2" customFormat="1" ht="325" customHeight="1" thickBot="1" x14ac:dyDescent="0.2">
-      <c r="A7" s="35"/>
-      <c r="B7" s="43"/>
+      <c r="A7" s="28"/>
+      <c r="B7" s="37"/>
       <c r="C7" s="20" t="s">
         <v>15</v>
       </c>
@@ -1366,16 +1369,16 @@
       <c r="AQ7"/>
     </row>
     <row r="8" spans="1:43" s="2" customFormat="1" ht="18" x14ac:dyDescent="0.15">
-      <c r="A8" s="36" t="s">
+      <c r="A8" s="30" t="s">
         <v>21</v>
       </c>
-      <c r="B8" s="37"/>
-      <c r="C8" s="37"/>
-      <c r="D8" s="37"/>
-      <c r="E8" s="37"/>
-      <c r="F8" s="37"/>
-      <c r="G8" s="37"/>
-      <c r="H8" s="38"/>
+      <c r="B8" s="31"/>
+      <c r="C8" s="31"/>
+      <c r="D8" s="31"/>
+      <c r="E8" s="31"/>
+      <c r="F8" s="31"/>
+      <c r="G8" s="31"/>
+      <c r="H8" s="32"/>
       <c r="I8"/>
       <c r="J8"/>
       <c r="K8"/>
@@ -1423,7 +1426,7 @@
       <c r="D9" s="24" t="s">
         <v>34</v>
       </c>
-      <c r="E9" s="48"/>
+      <c r="E9" s="26"/>
       <c r="F9" s="15"/>
       <c r="G9" s="15"/>
       <c r="H9" s="23"/>
@@ -1633,7 +1636,7 @@
       <c r="F13" s="24" t="s">
         <v>34</v>
       </c>
-      <c r="G13" s="47" t="s">
+      <c r="G13" s="25" t="s">
         <v>34</v>
       </c>
       <c r="H13" s="23"/>
@@ -1913,16 +1916,16 @@
       <c r="AQ18"/>
     </row>
     <row r="19" spans="1:43" s="2" customFormat="1" ht="18" x14ac:dyDescent="0.15">
-      <c r="A19" s="39" t="s">
+      <c r="A19" s="33" t="s">
         <v>22</v>
       </c>
-      <c r="B19" s="40"/>
-      <c r="C19" s="40"/>
-      <c r="D19" s="40"/>
-      <c r="E19" s="40"/>
-      <c r="F19" s="40"/>
-      <c r="G19" s="40"/>
-      <c r="H19" s="41"/>
+      <c r="B19" s="34"/>
+      <c r="C19" s="34"/>
+      <c r="D19" s="34"/>
+      <c r="E19" s="34"/>
+      <c r="F19" s="34"/>
+      <c r="G19" s="34"/>
+      <c r="H19" s="35"/>
       <c r="I19"/>
       <c r="J19"/>
       <c r="K19"/>
@@ -2293,16 +2296,16 @@
       <c r="AQ26"/>
     </row>
     <row r="27" spans="1:43" s="2" customFormat="1" ht="18" x14ac:dyDescent="0.15">
-      <c r="A27" s="39" t="s">
+      <c r="A27" s="33" t="s">
         <v>23</v>
       </c>
-      <c r="B27" s="40"/>
-      <c r="C27" s="40"/>
-      <c r="D27" s="40"/>
-      <c r="E27" s="40"/>
-      <c r="F27" s="40"/>
-      <c r="G27" s="40"/>
-      <c r="H27" s="41"/>
+      <c r="B27" s="34"/>
+      <c r="C27" s="34"/>
+      <c r="D27" s="34"/>
+      <c r="E27" s="34"/>
+      <c r="F27" s="34"/>
+      <c r="G27" s="34"/>
+      <c r="H27" s="35"/>
       <c r="I27"/>
       <c r="J27"/>
       <c r="K27"/>
@@ -2340,7 +2343,9 @@
       <c r="AQ27"/>
     </row>
     <row r="28" spans="1:43" s="2" customFormat="1" ht="40" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A28" s="9"/>
+      <c r="A28" s="9" t="s">
+        <v>48</v>
+      </c>
       <c r="B28" s="8"/>
       <c r="C28" s="15"/>
       <c r="D28" s="15"/>
@@ -2747,6 +2752,11 @@
     <row r="81" customFormat="1" x14ac:dyDescent="0.15"/>
   </sheetData>
   <mergeCells count="12">
+    <mergeCell ref="G1:H1"/>
+    <mergeCell ref="A1:F1"/>
+    <mergeCell ref="A3:E3"/>
+    <mergeCell ref="A4:E4"/>
+    <mergeCell ref="F3:H3"/>
     <mergeCell ref="A6:A7"/>
     <mergeCell ref="A2:H2"/>
     <mergeCell ref="A8:H8"/>
@@ -2754,11 +2764,6 @@
     <mergeCell ref="A27:H27"/>
     <mergeCell ref="B6:B7"/>
     <mergeCell ref="A5:H5"/>
-    <mergeCell ref="G1:H1"/>
-    <mergeCell ref="A1:F1"/>
-    <mergeCell ref="A3:E3"/>
-    <mergeCell ref="A4:E4"/>
-    <mergeCell ref="F3:H3"/>
   </mergeCells>
   <phoneticPr fontId="2" type="noConversion"/>
   <printOptions horizontalCentered="1" verticalCentered="1"/>
@@ -2770,6 +2775,26 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement>
+    <lcf76f155ced4ddcb4097134ff3c332f xmlns="44fce352-7b49-42d3-bc69-12da48d9ebc0">
+      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    </lcf76f155ced4ddcb4097134ff3c332f>
+    <TaxCatchAll xmlns="fbb90945-3c4c-43b7-bb15-9ae99079c100" xsi:nil="true"/>
+  </documentManagement>
+</p:properties>
+</file>
+
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x010100B44D25FE6749554FA89155DE40CE9E1E" ma:contentTypeVersion="14" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="8bb8039247b655a9c70bf36b5dd9dc64">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="44fce352-7b49-42d3-bc69-12da48d9ebc0" xmlns:ns3="fbb90945-3c4c-43b7-bb15-9ae99079c100" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="85d91c69c6e00024127dca24cda9fdf4" ns2:_="" ns3:_="">
     <xsd:import namespace="44fce352-7b49-42d3-bc69-12da48d9ebc0"/>
@@ -2998,27 +3023,32 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement>
-    <lcf76f155ced4ddcb4097134ff3c332f xmlns="44fce352-7b49-42d3-bc69-12da48d9ebc0">
-      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    </lcf76f155ced4ddcb4097134ff3c332f>
-    <TaxCatchAll xmlns="fbb90945-3c4c-43b7-bb15-9ae99079c100" xsi:nil="true"/>
-  </documentManagement>
-</p:properties>
+<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{4209C33D-ED08-404F-9B7A-29CD40C2ACA2}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
 
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{CD1FC233-9ECF-4A55-86D4-136E16072842}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="fbb90945-3c4c-43b7-bb15-9ae99079c100"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="44fce352-7b49-42d3-bc69-12da48d9ebc0"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
 
-<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{36ECBC65-C27A-4C6D-BAE3-04A998F6FAE4}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -3035,29 +3065,4 @@
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{CD1FC233-9ECF-4A55-86D4-136E16072842}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="fbb90945-3c4c-43b7-bb15-9ae99079c100"/>
-    <ds:schemaRef ds:uri="44fce352-7b49-42d3-bc69-12da48d9ebc0"/>
-    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
-    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{4209C33D-ED08-404F-9B7A-29CD40C2ACA2}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
 </file>
</xml_diff>

<commit_message>
tableau de synthese update
</commit_message>
<xml_diff>
--- a/assets/synthesegabriel.xlsx
+++ b/assets/synthesegabriel.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://testipformation-my.sharepoint.com/personal/g_martin_ecole-ipssi_net/Documents/IPSSI/Portfolio Final/assets/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="70" documentId="8_{11A09743-F9E9-41CF-B94B-EEA8224A8669}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{01E1C613-6F9C-274E-816B-4FD364ECBD60}"/>
+  <xr:revisionPtr revIDLastSave="101" documentId="8_{11A09743-F9E9-41CF-B94B-EEA8224A8669}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{3CC8A29F-4E4B-1640-8C68-C71A74753800}"/>
   <bookViews>
     <workbookView showHorizontalScroll="0" showVerticalScroll="0" showSheetTabs="0" xWindow="-20" yWindow="900" windowWidth="29400" windowHeight="16980" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -39,12 +39,9 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="62" uniqueCount="49">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="63" uniqueCount="49">
   <si>
     <t>BTS SERVICES INFORMATIQUES AUX ORGANISATIONS</t>
-  </si>
-  <si>
-    <t>SESSION 2024</t>
   </si>
   <si>
     <t xml:space="preserve">Tableau de synthèse des réalisations professionnelles </t>
@@ -138,9 +135,6 @@
     <t>Adresse URL du portfolio : https://fluffy1211.github.io/PortfolioGabriel/</t>
   </si>
   <si>
-    <t>Centre de formation : Ecole IPSSI</t>
-  </si>
-  <si>
     <t>Installation d'une VM Ubuntu</t>
   </si>
   <si>
@@ -159,20 +153,10 @@
     <t>06/05/24 au 26/05/24</t>
   </si>
   <si>
-    <t>Veilles informatiques</t>
-  </si>
-  <si>
     <t>X</t>
   </si>
   <si>
     <t>du 01/11/24 au 15/02/24</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Inventaire matériel réseau
-</t>
-  </si>
-  <si>
-    <t>Documentation GLPI</t>
   </si>
   <si>
     <t xml:space="preserve">Réalisation de mon Portfolio
@@ -189,25 +173,41 @@
 </t>
   </si>
   <si>
-    <t>le 16/09/2024</t>
-  </si>
-  <si>
-    <t>du 10/01/2023 au 05/06/2025</t>
-  </si>
-  <si>
-    <t>le 30/09/2024</t>
-  </si>
-  <si>
-    <t>du 16/09/2024 au 23/05/2024</t>
-  </si>
-  <si>
-    <t>du 08/01/2024 au 23/05/2024</t>
-  </si>
-  <si>
-    <t>du 10/04/2023 au 23/05/2024</t>
-  </si>
-  <si>
     <t>Création de de composant web</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Réalisation de l'Inventaire du matériel réseau
+</t>
+  </si>
+  <si>
+    <t>Mise en place d'outils de veilles informationnelles: google alerte/feedly</t>
+  </si>
+  <si>
+    <t>Installation et gestion des incidents avec GLPI</t>
+  </si>
+  <si>
+    <t>du 16/09/24 au 16/09/24</t>
+  </si>
+  <si>
+    <t>du 10/01/23 au 05/06/25</t>
+  </si>
+  <si>
+    <t>du 30/09/24 au 30/09/24</t>
+  </si>
+  <si>
+    <t>du 16/09/24 au 23/05/24</t>
+  </si>
+  <si>
+    <t>du 08/01/24 au 23/05/24</t>
+  </si>
+  <si>
+    <t>du 10/04/23 au 23/05/24</t>
+  </si>
+  <si>
+    <t>Centre de formation : IPSSI</t>
+  </si>
+  <si>
+    <t>SESSION 2025</t>
   </si>
 </sst>
 </file>
@@ -684,7 +684,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="164" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="49">
+  <cellXfs count="48">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="center"/>
@@ -759,9 +759,6 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="11" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -853,15 +850,15 @@
   <xdr:twoCellAnchor>
     <xdr:from>
       <xdr:col>7</xdr:col>
-      <xdr:colOff>228600</xdr:colOff>
+      <xdr:colOff>344355</xdr:colOff>
       <xdr:row>3</xdr:row>
-      <xdr:rowOff>203200</xdr:rowOff>
+      <xdr:rowOff>199893</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>7</xdr:col>
-      <xdr:colOff>342900</xdr:colOff>
+      <xdr:colOff>458655</xdr:colOff>
       <xdr:row>3</xdr:row>
-      <xdr:rowOff>330200</xdr:rowOff>
+      <xdr:rowOff>326893</xdr:rowOff>
     </xdr:to>
     <xdr:cxnSp macro="">
       <xdr:nvCxnSpPr>
@@ -876,7 +873,7 @@
       </xdr:nvCxnSpPr>
       <xdr:spPr>
         <a:xfrm flipV="1">
-          <a:off x="13817600" y="1739900"/>
+          <a:off x="15428912" y="1737784"/>
           <a:ext cx="114300" cy="127000"/>
         </a:xfrm>
         <a:prstGeom prst="line">
@@ -1199,8 +1196,8 @@
   </sheetPr>
   <dimension ref="A1:AQ81"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A12" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <selection activeCell="B28" sqref="B28"/>
+    <sheetView tabSelected="1" topLeftCell="A7" zoomScale="75" zoomScaleNormal="80" workbookViewId="0">
+      <selection activeCell="I5" sqref="I5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="10.83203125" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
@@ -1213,124 +1210,124 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:43" ht="40" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A1" s="29" t="s">
+      <c r="A1" s="28" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="29"/>
-      <c r="C1" s="29"/>
-      <c r="D1" s="29"/>
-      <c r="E1" s="29"/>
-      <c r="F1" s="29"/>
-      <c r="G1" s="29" t="s">
+      <c r="B1" s="28"/>
+      <c r="C1" s="28"/>
+      <c r="D1" s="28"/>
+      <c r="E1" s="28"/>
+      <c r="F1" s="28"/>
+      <c r="G1" s="28" t="s">
+        <v>48</v>
+      </c>
+      <c r="H1" s="28"/>
+    </row>
+    <row r="2" spans="1:43" ht="41" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A2" s="28" t="s">
         <v>1</v>
       </c>
-      <c r="H1" s="29"/>
-    </row>
-    <row r="2" spans="1:43" ht="41" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A2" s="29" t="s">
+      <c r="B2" s="28"/>
+      <c r="C2" s="28"/>
+      <c r="D2" s="28"/>
+      <c r="E2" s="28"/>
+      <c r="F2" s="28"/>
+      <c r="G2" s="28"/>
+      <c r="H2" s="28"/>
+    </row>
+    <row r="3" spans="1:43" ht="40" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A3" s="40" t="s">
+        <v>23</v>
+      </c>
+      <c r="B3" s="41"/>
+      <c r="C3" s="41"/>
+      <c r="D3" s="41"/>
+      <c r="E3" s="42"/>
+      <c r="F3" s="46" t="s">
         <v>2</v>
       </c>
-      <c r="B2" s="29"/>
-      <c r="C2" s="29"/>
-      <c r="D2" s="29"/>
-      <c r="E2" s="29"/>
-      <c r="F2" s="29"/>
-      <c r="G2" s="29"/>
-      <c r="H2" s="29"/>
-    </row>
-    <row r="3" spans="1:43" ht="40" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A3" s="41" t="s">
-        <v>24</v>
-      </c>
-      <c r="B3" s="42"/>
-      <c r="C3" s="42"/>
-      <c r="D3" s="42"/>
-      <c r="E3" s="43"/>
-      <c r="F3" s="47" t="s">
-        <v>3</v>
-      </c>
-      <c r="G3" s="42"/>
-      <c r="H3" s="48"/>
+      <c r="G3" s="41"/>
+      <c r="H3" s="47"/>
       <c r="K3" s="1"/>
       <c r="L3" s="1"/>
       <c r="M3" s="1"/>
     </row>
     <row r="4" spans="1:43" ht="40" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A4" s="44" t="s">
-        <v>26</v>
-      </c>
-      <c r="B4" s="45"/>
-      <c r="C4" s="45"/>
-      <c r="D4" s="45"/>
-      <c r="E4" s="46"/>
+      <c r="A4" s="43" t="s">
+        <v>47</v>
+      </c>
+      <c r="B4" s="44"/>
+      <c r="C4" s="44"/>
+      <c r="D4" s="44"/>
+      <c r="E4" s="45"/>
       <c r="F4" s="12" t="s">
+        <v>3</v>
+      </c>
+      <c r="G4" s="13" t="s">
         <v>4</v>
       </c>
-      <c r="G4" s="13" t="s">
+      <c r="H4" s="19" t="s">
         <v>5</v>
       </c>
-      <c r="H4" s="19" t="s">
+    </row>
+    <row r="5" spans="1:43" ht="40" customHeight="1" thickBot="1" x14ac:dyDescent="0.2">
+      <c r="A5" s="37" t="s">
+        <v>24</v>
+      </c>
+      <c r="B5" s="38"/>
+      <c r="C5" s="38"/>
+      <c r="D5" s="38"/>
+      <c r="E5" s="38"/>
+      <c r="F5" s="38"/>
+      <c r="G5" s="38"/>
+      <c r="H5" s="39"/>
+    </row>
+    <row r="6" spans="1:43" ht="90" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A6" s="26" t="s">
         <v>6</v>
       </c>
-    </row>
-    <row r="5" spans="1:43" ht="40" customHeight="1" thickBot="1" x14ac:dyDescent="0.2">
-      <c r="A5" s="38" t="s">
-        <v>25</v>
-      </c>
-      <c r="B5" s="39"/>
-      <c r="C5" s="39"/>
-      <c r="D5" s="39"/>
-      <c r="E5" s="39"/>
-      <c r="F5" s="39"/>
-      <c r="G5" s="39"/>
-      <c r="H5" s="40"/>
-    </row>
-    <row r="6" spans="1:43" ht="90" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A6" s="27" t="s">
+      <c r="B6" s="35" t="s">
         <v>7</v>
       </c>
-      <c r="B6" s="36" t="s">
+      <c r="C6" s="6" t="s">
         <v>8</v>
       </c>
-      <c r="C6" s="6" t="s">
+      <c r="D6" s="6" t="s">
         <v>9</v>
       </c>
-      <c r="D6" s="6" t="s">
+      <c r="E6" s="6" t="s">
         <v>10</v>
       </c>
-      <c r="E6" s="6" t="s">
+      <c r="F6" s="6" t="s">
         <v>11</v>
       </c>
-      <c r="F6" s="6" t="s">
+      <c r="G6" s="6" t="s">
         <v>12</v>
       </c>
-      <c r="G6" s="6" t="s">
+      <c r="H6" s="7" t="s">
         <v>13</v>
       </c>
-      <c r="H6" s="7" t="s">
+    </row>
+    <row r="7" spans="1:43" s="2" customFormat="1" ht="325" customHeight="1" thickBot="1" x14ac:dyDescent="0.2">
+      <c r="A7" s="27"/>
+      <c r="B7" s="36"/>
+      <c r="C7" s="20" t="s">
         <v>14</v>
       </c>
-    </row>
-    <row r="7" spans="1:43" s="2" customFormat="1" ht="325" customHeight="1" thickBot="1" x14ac:dyDescent="0.2">
-      <c r="A7" s="28"/>
-      <c r="B7" s="37"/>
-      <c r="C7" s="20" t="s">
+      <c r="D7" s="20" t="s">
         <v>15</v>
       </c>
-      <c r="D7" s="20" t="s">
+      <c r="E7" s="20" t="s">
         <v>16</v>
       </c>
-      <c r="E7" s="20" t="s">
+      <c r="F7" s="20" t="s">
         <v>17</v>
       </c>
-      <c r="F7" s="20" t="s">
+      <c r="G7" s="20" t="s">
         <v>18</v>
       </c>
-      <c r="G7" s="20" t="s">
+      <c r="H7" s="21" t="s">
         <v>19</v>
-      </c>
-      <c r="H7" s="21" t="s">
-        <v>20</v>
       </c>
       <c r="I7"/>
       <c r="J7"/>
@@ -1369,16 +1366,16 @@
       <c r="AQ7"/>
     </row>
     <row r="8" spans="1:43" s="2" customFormat="1" ht="18" x14ac:dyDescent="0.15">
-      <c r="A8" s="30" t="s">
-        <v>21</v>
-      </c>
-      <c r="B8" s="31"/>
-      <c r="C8" s="31"/>
-      <c r="D8" s="31"/>
-      <c r="E8" s="31"/>
-      <c r="F8" s="31"/>
-      <c r="G8" s="31"/>
-      <c r="H8" s="32"/>
+      <c r="A8" s="29" t="s">
+        <v>20</v>
+      </c>
+      <c r="B8" s="30"/>
+      <c r="C8" s="30"/>
+      <c r="D8" s="30"/>
+      <c r="E8" s="30"/>
+      <c r="F8" s="30"/>
+      <c r="G8" s="30"/>
+      <c r="H8" s="31"/>
       <c r="I8"/>
       <c r="J8"/>
       <c r="K8"/>
@@ -1417,16 +1414,16 @@
     </row>
     <row r="9" spans="1:43" s="2" customFormat="1" ht="40" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A9" s="9" t="s">
-        <v>39</v>
+        <v>34</v>
       </c>
       <c r="B9" s="8" t="s">
-        <v>35</v>
+        <v>32</v>
       </c>
       <c r="C9" s="14"/>
-      <c r="D9" s="24" t="s">
-        <v>34</v>
-      </c>
-      <c r="E9" s="26"/>
+      <c r="D9" s="24"/>
+      <c r="E9" s="24" t="s">
+        <v>31</v>
+      </c>
       <c r="F9" s="15"/>
       <c r="G9" s="15"/>
       <c r="H9" s="23"/>
@@ -1468,13 +1465,13 @@
     </row>
     <row r="10" spans="1:43" s="2" customFormat="1" ht="40" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A10" s="9" t="s">
-        <v>36</v>
+        <v>38</v>
       </c>
       <c r="B10" s="8" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="C10" s="24" t="s">
-        <v>34</v>
+        <v>31</v>
       </c>
       <c r="D10" s="15"/>
       <c r="E10" s="15"/>
@@ -1519,10 +1516,10 @@
     </row>
     <row r="11" spans="1:43" s="2" customFormat="1" ht="40" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A11" s="9" t="s">
-        <v>33</v>
+        <v>39</v>
       </c>
       <c r="B11" s="8" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="C11" s="15"/>
       <c r="D11" s="15"/>
@@ -1530,7 +1527,7 @@
       <c r="F11" s="15"/>
       <c r="G11" s="15"/>
       <c r="H11" s="23" t="s">
-        <v>34</v>
+        <v>31</v>
       </c>
       <c r="I11"/>
       <c r="J11"/>
@@ -1570,21 +1567,21 @@
     </row>
     <row r="12" spans="1:43" s="2" customFormat="1" ht="40" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A12" s="9" t="s">
-        <v>37</v>
+        <v>40</v>
       </c>
       <c r="B12" s="8" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="C12" s="24" t="s">
-        <v>34</v>
+        <v>31</v>
       </c>
       <c r="D12" s="24" t="s">
-        <v>34</v>
+        <v>31</v>
       </c>
       <c r="E12" s="15"/>
       <c r="F12" s="24"/>
       <c r="G12" s="24" t="s">
-        <v>34</v>
+        <v>31</v>
       </c>
       <c r="H12" s="16"/>
       <c r="I12"/>
@@ -1625,19 +1622,19 @@
     </row>
     <row r="13" spans="1:43" s="2" customFormat="1" ht="40" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A13" s="9" t="s">
-        <v>40</v>
+        <v>35</v>
       </c>
       <c r="B13" s="8" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="C13" s="15"/>
       <c r="D13" s="15"/>
       <c r="E13" s="15"/>
       <c r="F13" s="24" t="s">
-        <v>34</v>
+        <v>31</v>
       </c>
       <c r="G13" s="25" t="s">
-        <v>34</v>
+        <v>31</v>
       </c>
       <c r="H13" s="23"/>
       <c r="I13"/>
@@ -1678,23 +1675,21 @@
     </row>
     <row r="14" spans="1:43" s="2" customFormat="1" ht="40" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A14" s="9" t="s">
-        <v>41</v>
+        <v>36</v>
       </c>
       <c r="B14" s="8" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="C14" s="15"/>
       <c r="D14" s="15"/>
       <c r="E14" s="15"/>
       <c r="F14" s="24" t="s">
-        <v>34</v>
+        <v>31</v>
       </c>
       <c r="G14" s="24" t="s">
-        <v>34</v>
-      </c>
-      <c r="H14" s="23" t="s">
-        <v>34</v>
-      </c>
+        <v>31</v>
+      </c>
+      <c r="H14" s="23"/>
       <c r="I14"/>
       <c r="J14"/>
       <c r="K14"/>
@@ -1733,17 +1728,19 @@
     </row>
     <row r="15" spans="1:43" s="2" customFormat="1" ht="40" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A15" s="9" t="s">
-        <v>38</v>
+        <v>33</v>
       </c>
       <c r="B15" s="8" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="C15" s="15"/>
       <c r="D15" s="15"/>
       <c r="E15" s="15"/>
       <c r="F15" s="15"/>
       <c r="G15" s="15"/>
-      <c r="H15" s="16"/>
+      <c r="H15" s="23" t="s">
+        <v>31</v>
+      </c>
       <c r="I15"/>
       <c r="J15"/>
       <c r="K15"/>
@@ -1785,7 +1782,9 @@
       <c r="B16" s="8"/>
       <c r="C16" s="15"/>
       <c r="D16" s="15"/>
-      <c r="E16" s="15"/>
+      <c r="E16" s="24" t="s">
+        <v>31</v>
+      </c>
       <c r="F16" s="15"/>
       <c r="G16" s="15"/>
       <c r="H16" s="16"/>
@@ -1830,7 +1829,6 @@
       <c r="B17" s="8"/>
       <c r="C17" s="15"/>
       <c r="D17" s="15"/>
-      <c r="E17" s="15"/>
       <c r="F17" s="15"/>
       <c r="G17" s="15"/>
       <c r="H17" s="16"/>
@@ -1916,16 +1914,16 @@
       <c r="AQ18"/>
     </row>
     <row r="19" spans="1:43" s="2" customFormat="1" ht="18" x14ac:dyDescent="0.15">
-      <c r="A19" s="33" t="s">
-        <v>22</v>
-      </c>
-      <c r="B19" s="34"/>
-      <c r="C19" s="34"/>
-      <c r="D19" s="34"/>
-      <c r="E19" s="34"/>
-      <c r="F19" s="34"/>
-      <c r="G19" s="34"/>
-      <c r="H19" s="35"/>
+      <c r="A19" s="32" t="s">
+        <v>21</v>
+      </c>
+      <c r="B19" s="33"/>
+      <c r="C19" s="33"/>
+      <c r="D19" s="33"/>
+      <c r="E19" s="33"/>
+      <c r="F19" s="33"/>
+      <c r="G19" s="33"/>
+      <c r="H19" s="34"/>
       <c r="I19"/>
       <c r="J19"/>
       <c r="K19"/>
@@ -1964,17 +1962,17 @@
     </row>
     <row r="20" spans="1:43" s="2" customFormat="1" ht="40" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A20" s="9" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
       <c r="B20" s="22" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="C20" s="15"/>
       <c r="D20" s="15"/>
       <c r="E20" s="15"/>
       <c r="F20" s="15"/>
       <c r="G20" s="24" t="s">
-        <v>34</v>
+        <v>31</v>
       </c>
       <c r="H20" s="16"/>
       <c r="I20"/>
@@ -2015,17 +2013,17 @@
     </row>
     <row r="21" spans="1:43" s="2" customFormat="1" ht="40" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A21" s="9" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
       <c r="B21" s="8" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="C21" s="15"/>
       <c r="D21" s="15"/>
       <c r="E21" s="15"/>
       <c r="F21" s="15"/>
       <c r="G21" s="24" t="s">
-        <v>34</v>
+        <v>31</v>
       </c>
       <c r="H21" s="16"/>
       <c r="I21"/>
@@ -2066,15 +2064,15 @@
     </row>
     <row r="22" spans="1:43" s="2" customFormat="1" ht="40" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A22" s="9" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="B22" s="8" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
       <c r="C22" s="15"/>
       <c r="D22" s="15"/>
       <c r="E22" s="24" t="s">
-        <v>34</v>
+        <v>31</v>
       </c>
       <c r="F22" s="15"/>
       <c r="G22" s="15"/>
@@ -2296,16 +2294,16 @@
       <c r="AQ26"/>
     </row>
     <row r="27" spans="1:43" s="2" customFormat="1" ht="18" x14ac:dyDescent="0.15">
-      <c r="A27" s="33" t="s">
-        <v>23</v>
-      </c>
-      <c r="B27" s="34"/>
-      <c r="C27" s="34"/>
-      <c r="D27" s="34"/>
-      <c r="E27" s="34"/>
-      <c r="F27" s="34"/>
-      <c r="G27" s="34"/>
-      <c r="H27" s="35"/>
+      <c r="A27" s="32" t="s">
+        <v>22</v>
+      </c>
+      <c r="B27" s="33"/>
+      <c r="C27" s="33"/>
+      <c r="D27" s="33"/>
+      <c r="E27" s="33"/>
+      <c r="F27" s="33"/>
+      <c r="G27" s="33"/>
+      <c r="H27" s="34"/>
       <c r="I27"/>
       <c r="J27"/>
       <c r="K27"/>
@@ -2344,7 +2342,7 @@
     </row>
     <row r="28" spans="1:43" s="2" customFormat="1" ht="40" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A28" s="9" t="s">
-        <v>48</v>
+        <v>37</v>
       </c>
       <c r="B28" s="8"/>
       <c r="C28" s="15"/>

</xml_diff>

<commit_message>
Update styles and content in index.html and style.css
</commit_message>
<xml_diff>
--- a/assets/synthesegabriel.xlsx
+++ b/assets/synthesegabriel.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://testipformation-my.sharepoint.com/personal/g_martin_ecole-ipssi_net/Documents/IPSSI/Portfolio Final/assets/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="101" documentId="8_{11A09743-F9E9-41CF-B94B-EEA8224A8669}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{3CC8A29F-4E4B-1640-8C68-C71A74753800}"/>
+  <xr:revisionPtr revIDLastSave="114" documentId="8_{11A09743-F9E9-41CF-B94B-EEA8224A8669}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{43F02026-3072-5042-9497-A217613DD590}"/>
   <bookViews>
-    <workbookView showHorizontalScroll="0" showVerticalScroll="0" showSheetTabs="0" xWindow="-20" yWindow="900" windowWidth="29400" windowHeight="16980" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView showHorizontalScroll="0" showVerticalScroll="0" showSheetTabs="0" xWindow="0" yWindow="900" windowWidth="29400" windowHeight="16980" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Tableau de synthèse Épreuve E4" sheetId="1" r:id="rId1"/>
@@ -39,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="63" uniqueCount="49">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="70" uniqueCount="53">
   <si>
     <t>BTS SERVICES INFORMATIQUES AUX ORGANISATIONS</t>
   </si>
@@ -144,9 +144,6 @@
     <t>Maintenance d'une application web</t>
   </si>
   <si>
-    <t>17/06/2024 au 19/06/24</t>
-  </si>
-  <si>
     <t>19/06/24 au 22/06/24</t>
   </si>
   <si>
@@ -208,6 +205,21 @@
   </si>
   <si>
     <t>SESSION 2025</t>
+  </si>
+  <si>
+    <t>Collaboration grâce à la méthode SCRUM</t>
+  </si>
+  <si>
+    <t>01/12/24 au 15/12/24</t>
+  </si>
+  <si>
+    <t>17/06/24 au 19/06/24</t>
+  </si>
+  <si>
+    <t>09/09/24 au 15/05/24</t>
+  </si>
+  <si>
+    <t>09/09/24 au 20/12/24</t>
   </si>
 </sst>
 </file>
@@ -1196,8 +1208,8 @@
   </sheetPr>
   <dimension ref="A1:AQ81"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A7" zoomScale="75" zoomScaleNormal="80" workbookViewId="0">
-      <selection activeCell="I5" sqref="I5"/>
+    <sheetView tabSelected="1" topLeftCell="A16" zoomScale="75" zoomScaleNormal="80" workbookViewId="0">
+      <selection activeCell="E28" sqref="E28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="10.83203125" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
@@ -1219,7 +1231,7 @@
       <c r="E1" s="28"/>
       <c r="F1" s="28"/>
       <c r="G1" s="28" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="H1" s="28"/>
     </row>
@@ -1254,7 +1266,7 @@
     </row>
     <row r="4" spans="1:43" ht="40" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A4" s="43" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="B4" s="44"/>
       <c r="C4" s="44"/>
@@ -1414,15 +1426,15 @@
     </row>
     <row r="9" spans="1:43" s="2" customFormat="1" ht="40" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A9" s="9" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="B9" s="8" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="C9" s="14"/>
       <c r="D9" s="24"/>
       <c r="E9" s="24" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="F9" s="15"/>
       <c r="G9" s="15"/>
@@ -1465,13 +1477,13 @@
     </row>
     <row r="10" spans="1:43" s="2" customFormat="1" ht="40" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A10" s="9" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="B10" s="8" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="C10" s="24" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="D10" s="15"/>
       <c r="E10" s="15"/>
@@ -1516,10 +1528,10 @@
     </row>
     <row r="11" spans="1:43" s="2" customFormat="1" ht="40" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A11" s="9" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="B11" s="8" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="C11" s="15"/>
       <c r="D11" s="15"/>
@@ -1527,7 +1539,7 @@
       <c r="F11" s="15"/>
       <c r="G11" s="15"/>
       <c r="H11" s="23" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="I11"/>
       <c r="J11"/>
@@ -1567,21 +1579,21 @@
     </row>
     <row r="12" spans="1:43" s="2" customFormat="1" ht="40" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A12" s="9" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="B12" s="8" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="C12" s="24" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="D12" s="24" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="E12" s="15"/>
       <c r="F12" s="24"/>
       <c r="G12" s="24" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="H12" s="16"/>
       <c r="I12"/>
@@ -1622,19 +1634,19 @@
     </row>
     <row r="13" spans="1:43" s="2" customFormat="1" ht="40" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A13" s="9" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="B13" s="8" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="C13" s="15"/>
       <c r="D13" s="15"/>
       <c r="E13" s="15"/>
       <c r="F13" s="24" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="G13" s="25" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="H13" s="23"/>
       <c r="I13"/>
@@ -1675,19 +1687,19 @@
     </row>
     <row r="14" spans="1:43" s="2" customFormat="1" ht="40" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A14" s="9" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="B14" s="8" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="C14" s="15"/>
       <c r="D14" s="15"/>
       <c r="E14" s="15"/>
       <c r="F14" s="24" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="G14" s="24" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="H14" s="23"/>
       <c r="I14"/>
@@ -1728,10 +1740,10 @@
     </row>
     <row r="15" spans="1:43" s="2" customFormat="1" ht="40" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A15" s="9" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="B15" s="8" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="C15" s="15"/>
       <c r="D15" s="15"/>
@@ -1739,7 +1751,7 @@
       <c r="F15" s="15"/>
       <c r="G15" s="15"/>
       <c r="H15" s="23" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="I15"/>
       <c r="J15"/>
@@ -1782,9 +1794,7 @@
       <c r="B16" s="8"/>
       <c r="C16" s="15"/>
       <c r="D16" s="15"/>
-      <c r="E16" s="24" t="s">
-        <v>31</v>
-      </c>
+      <c r="E16" s="24"/>
       <c r="F16" s="15"/>
       <c r="G16" s="15"/>
       <c r="H16" s="16"/>
@@ -1965,14 +1975,14 @@
         <v>25</v>
       </c>
       <c r="B20" s="22" t="s">
-        <v>28</v>
+        <v>50</v>
       </c>
       <c r="C20" s="15"/>
       <c r="D20" s="15"/>
       <c r="E20" s="15"/>
       <c r="F20" s="15"/>
       <c r="G20" s="24" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="H20" s="16"/>
       <c r="I20"/>
@@ -2016,14 +2026,14 @@
         <v>26</v>
       </c>
       <c r="B21" s="8" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="C21" s="15"/>
       <c r="D21" s="15"/>
       <c r="E21" s="15"/>
       <c r="F21" s="15"/>
       <c r="G21" s="24" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="H21" s="16"/>
       <c r="I21"/>
@@ -2067,12 +2077,12 @@
         <v>27</v>
       </c>
       <c r="B22" s="8" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="C22" s="15"/>
       <c r="D22" s="15"/>
       <c r="E22" s="24" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="F22" s="15"/>
       <c r="G22" s="15"/>
@@ -2342,12 +2352,16 @@
     </row>
     <row r="28" spans="1:43" s="2" customFormat="1" ht="40" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A28" s="9" t="s">
-        <v>37</v>
-      </c>
-      <c r="B28" s="8"/>
+        <v>36</v>
+      </c>
+      <c r="B28" s="8" t="s">
+        <v>49</v>
+      </c>
       <c r="C28" s="15"/>
       <c r="D28" s="15"/>
-      <c r="E28" s="15"/>
+      <c r="E28" s="24" t="s">
+        <v>30</v>
+      </c>
       <c r="F28" s="15"/>
       <c r="G28" s="15"/>
       <c r="H28" s="16"/>
@@ -2388,11 +2402,17 @@
       <c r="AQ28"/>
     </row>
     <row r="29" spans="1:43" s="2" customFormat="1" ht="40" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A29" s="9"/>
-      <c r="B29" s="8"/>
+      <c r="A29" s="9" t="s">
+        <v>27</v>
+      </c>
+      <c r="B29" s="8" t="s">
+        <v>52</v>
+      </c>
       <c r="C29" s="15"/>
       <c r="D29" s="15"/>
-      <c r="E29" s="15"/>
+      <c r="E29" s="24" t="s">
+        <v>30</v>
+      </c>
       <c r="F29" s="15"/>
       <c r="G29" s="15"/>
       <c r="H29" s="16"/>
@@ -2433,12 +2453,18 @@
       <c r="AQ29"/>
     </row>
     <row r="30" spans="1:43" s="2" customFormat="1" ht="40" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A30" s="9"/>
-      <c r="B30" s="8"/>
+      <c r="A30" s="9" t="s">
+        <v>48</v>
+      </c>
+      <c r="B30" s="8" t="s">
+        <v>51</v>
+      </c>
       <c r="C30" s="15"/>
       <c r="D30" s="15"/>
       <c r="E30" s="15"/>
-      <c r="F30" s="15"/>
+      <c r="F30" s="24" t="s">
+        <v>30</v>
+      </c>
       <c r="G30" s="15"/>
       <c r="H30" s="16"/>
       <c r="I30"/>
@@ -3032,16 +3058,16 @@
 <file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{CD1FC233-9ECF-4A55-86D4-136E16072842}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="fbb90945-3c4c-43b7-bb15-9ae99079c100"/>
+    <ds:schemaRef ds:uri="44fce352-7b49-42d3-bc69-12da48d9ebc0"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
     <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
     <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
     <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
-    <ds:schemaRef ds:uri="44fce352-7b49-42d3-bc69-12da48d9ebc0"/>
-    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="fbb90945-3c4c-43b7-bb15-9ae99079c100"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>

</xml_diff>

<commit_message>
Update links to open in new tabs and modify content in index.html
</commit_message>
<xml_diff>
--- a/assets/synthesegabriel.xlsx
+++ b/assets/synthesegabriel.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://testipformation-my.sharepoint.com/personal/g_martin_ecole-ipssi_net/Documents/IPSSI/Portfolio Final/assets/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="114" documentId="8_{11A09743-F9E9-41CF-B94B-EEA8224A8669}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{43F02026-3072-5042-9497-A217613DD590}"/>
+  <xr:revisionPtr revIDLastSave="115" documentId="8_{11A09743-F9E9-41CF-B94B-EEA8224A8669}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{A9C8E924-67C5-3645-A5C6-616B7D840A1C}"/>
   <bookViews>
     <workbookView showHorizontalScroll="0" showVerticalScroll="0" showSheetTabs="0" xWindow="0" yWindow="900" windowWidth="29400" windowHeight="16980" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -195,9 +195,6 @@
     <t>du 16/09/24 au 23/05/24</t>
   </si>
   <si>
-    <t>du 08/01/24 au 23/05/24</t>
-  </si>
-  <si>
     <t>du 10/04/23 au 23/05/24</t>
   </si>
   <si>
@@ -220,6 +217,9 @@
   </si>
   <si>
     <t>09/09/24 au 20/12/24</t>
+  </si>
+  <si>
+    <t>du 08/01/25 au 23/05/25</t>
   </si>
 </sst>
 </file>
@@ -773,15 +773,39 @@
     <xf numFmtId="0" fontId="11" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="20" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="21" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="22" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="25" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="23" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="24" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -813,30 +837,6 @@
       <alignment horizontal="left" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="28" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="20" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="21" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="22" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="25" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="23" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="24" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
   </cellXfs>
@@ -1208,8 +1208,8 @@
   </sheetPr>
   <dimension ref="A1:AQ81"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A16" zoomScale="75" zoomScaleNormal="80" workbookViewId="0">
-      <selection activeCell="E28" sqref="E28"/>
+    <sheetView tabSelected="1" topLeftCell="A6" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
+      <selection activeCell="F13" sqref="F13:G14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="10.83203125" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
@@ -1222,56 +1222,56 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:43" ht="40" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A1" s="28" t="s">
+      <c r="A1" s="26" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="28"/>
-      <c r="C1" s="28"/>
-      <c r="D1" s="28"/>
-      <c r="E1" s="28"/>
-      <c r="F1" s="28"/>
-      <c r="G1" s="28" t="s">
-        <v>47</v>
-      </c>
-      <c r="H1" s="28"/>
+      <c r="B1" s="26"/>
+      <c r="C1" s="26"/>
+      <c r="D1" s="26"/>
+      <c r="E1" s="26"/>
+      <c r="F1" s="26"/>
+      <c r="G1" s="26" t="s">
+        <v>46</v>
+      </c>
+      <c r="H1" s="26"/>
     </row>
     <row r="2" spans="1:43" ht="41" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A2" s="28" t="s">
+      <c r="A2" s="26" t="s">
         <v>1</v>
       </c>
-      <c r="B2" s="28"/>
-      <c r="C2" s="28"/>
-      <c r="D2" s="28"/>
-      <c r="E2" s="28"/>
-      <c r="F2" s="28"/>
-      <c r="G2" s="28"/>
-      <c r="H2" s="28"/>
+      <c r="B2" s="26"/>
+      <c r="C2" s="26"/>
+      <c r="D2" s="26"/>
+      <c r="E2" s="26"/>
+      <c r="F2" s="26"/>
+      <c r="G2" s="26"/>
+      <c r="H2" s="26"/>
     </row>
     <row r="3" spans="1:43" ht="40" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A3" s="40" t="s">
+      <c r="A3" s="27" t="s">
         <v>23</v>
       </c>
-      <c r="B3" s="41"/>
-      <c r="C3" s="41"/>
-      <c r="D3" s="41"/>
-      <c r="E3" s="42"/>
-      <c r="F3" s="46" t="s">
+      <c r="B3" s="28"/>
+      <c r="C3" s="28"/>
+      <c r="D3" s="28"/>
+      <c r="E3" s="29"/>
+      <c r="F3" s="33" t="s">
         <v>2</v>
       </c>
-      <c r="G3" s="41"/>
-      <c r="H3" s="47"/>
+      <c r="G3" s="28"/>
+      <c r="H3" s="34"/>
       <c r="K3" s="1"/>
       <c r="L3" s="1"/>
       <c r="M3" s="1"/>
     </row>
     <row r="4" spans="1:43" ht="40" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A4" s="43" t="s">
-        <v>46</v>
-      </c>
-      <c r="B4" s="44"/>
-      <c r="C4" s="44"/>
-      <c r="D4" s="44"/>
-      <c r="E4" s="45"/>
+      <c r="A4" s="30" t="s">
+        <v>45</v>
+      </c>
+      <c r="B4" s="31"/>
+      <c r="C4" s="31"/>
+      <c r="D4" s="31"/>
+      <c r="E4" s="32"/>
       <c r="F4" s="12" t="s">
         <v>3</v>
       </c>
@@ -1283,22 +1283,22 @@
       </c>
     </row>
     <row r="5" spans="1:43" ht="40" customHeight="1" thickBot="1" x14ac:dyDescent="0.2">
-      <c r="A5" s="37" t="s">
+      <c r="A5" s="45" t="s">
         <v>24</v>
       </c>
-      <c r="B5" s="38"/>
-      <c r="C5" s="38"/>
-      <c r="D5" s="38"/>
-      <c r="E5" s="38"/>
-      <c r="F5" s="38"/>
-      <c r="G5" s="38"/>
-      <c r="H5" s="39"/>
+      <c r="B5" s="46"/>
+      <c r="C5" s="46"/>
+      <c r="D5" s="46"/>
+      <c r="E5" s="46"/>
+      <c r="F5" s="46"/>
+      <c r="G5" s="46"/>
+      <c r="H5" s="47"/>
     </row>
     <row r="6" spans="1:43" ht="90" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A6" s="26" t="s">
+      <c r="A6" s="35" t="s">
         <v>6</v>
       </c>
-      <c r="B6" s="35" t="s">
+      <c r="B6" s="43" t="s">
         <v>7</v>
       </c>
       <c r="C6" s="6" t="s">
@@ -1321,8 +1321,8 @@
       </c>
     </row>
     <row r="7" spans="1:43" s="2" customFormat="1" ht="325" customHeight="1" thickBot="1" x14ac:dyDescent="0.2">
-      <c r="A7" s="27"/>
-      <c r="B7" s="36"/>
+      <c r="A7" s="36"/>
+      <c r="B7" s="44"/>
       <c r="C7" s="20" t="s">
         <v>14</v>
       </c>
@@ -1378,16 +1378,16 @@
       <c r="AQ7"/>
     </row>
     <row r="8" spans="1:43" s="2" customFormat="1" ht="18" x14ac:dyDescent="0.15">
-      <c r="A8" s="29" t="s">
+      <c r="A8" s="37" t="s">
         <v>20</v>
       </c>
-      <c r="B8" s="30"/>
-      <c r="C8" s="30"/>
-      <c r="D8" s="30"/>
-      <c r="E8" s="30"/>
-      <c r="F8" s="30"/>
-      <c r="G8" s="30"/>
-      <c r="H8" s="31"/>
+      <c r="B8" s="38"/>
+      <c r="C8" s="38"/>
+      <c r="D8" s="38"/>
+      <c r="E8" s="38"/>
+      <c r="F8" s="38"/>
+      <c r="G8" s="38"/>
+      <c r="H8" s="39"/>
       <c r="I8"/>
       <c r="J8"/>
       <c r="K8"/>
@@ -1690,7 +1690,7 @@
         <v>35</v>
       </c>
       <c r="B14" s="8" t="s">
-        <v>44</v>
+        <v>52</v>
       </c>
       <c r="C14" s="15"/>
       <c r="D14" s="15"/>
@@ -1743,7 +1743,7 @@
         <v>32</v>
       </c>
       <c r="B15" s="8" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="C15" s="15"/>
       <c r="D15" s="15"/>
@@ -1924,16 +1924,16 @@
       <c r="AQ18"/>
     </row>
     <row r="19" spans="1:43" s="2" customFormat="1" ht="18" x14ac:dyDescent="0.15">
-      <c r="A19" s="32" t="s">
+      <c r="A19" s="40" t="s">
         <v>21</v>
       </c>
-      <c r="B19" s="33"/>
-      <c r="C19" s="33"/>
-      <c r="D19" s="33"/>
-      <c r="E19" s="33"/>
-      <c r="F19" s="33"/>
-      <c r="G19" s="33"/>
-      <c r="H19" s="34"/>
+      <c r="B19" s="41"/>
+      <c r="C19" s="41"/>
+      <c r="D19" s="41"/>
+      <c r="E19" s="41"/>
+      <c r="F19" s="41"/>
+      <c r="G19" s="41"/>
+      <c r="H19" s="42"/>
       <c r="I19"/>
       <c r="J19"/>
       <c r="K19"/>
@@ -1975,7 +1975,7 @@
         <v>25</v>
       </c>
       <c r="B20" s="22" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="C20" s="15"/>
       <c r="D20" s="15"/>
@@ -2304,16 +2304,16 @@
       <c r="AQ26"/>
     </row>
     <row r="27" spans="1:43" s="2" customFormat="1" ht="18" x14ac:dyDescent="0.15">
-      <c r="A27" s="32" t="s">
+      <c r="A27" s="40" t="s">
         <v>22</v>
       </c>
-      <c r="B27" s="33"/>
-      <c r="C27" s="33"/>
-      <c r="D27" s="33"/>
-      <c r="E27" s="33"/>
-      <c r="F27" s="33"/>
-      <c r="G27" s="33"/>
-      <c r="H27" s="34"/>
+      <c r="B27" s="41"/>
+      <c r="C27" s="41"/>
+      <c r="D27" s="41"/>
+      <c r="E27" s="41"/>
+      <c r="F27" s="41"/>
+      <c r="G27" s="41"/>
+      <c r="H27" s="42"/>
       <c r="I27"/>
       <c r="J27"/>
       <c r="K27"/>
@@ -2355,7 +2355,7 @@
         <v>36</v>
       </c>
       <c r="B28" s="8" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="C28" s="15"/>
       <c r="D28" s="15"/>
@@ -2406,7 +2406,7 @@
         <v>27</v>
       </c>
       <c r="B29" s="8" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="C29" s="15"/>
       <c r="D29" s="15"/>
@@ -2454,10 +2454,10 @@
     </row>
     <row r="30" spans="1:43" s="2" customFormat="1" ht="40" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A30" s="9" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="B30" s="8" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="C30" s="15"/>
       <c r="D30" s="15"/>
@@ -2776,11 +2776,6 @@
     <row r="81" customFormat="1" x14ac:dyDescent="0.15"/>
   </sheetData>
   <mergeCells count="12">
-    <mergeCell ref="G1:H1"/>
-    <mergeCell ref="A1:F1"/>
-    <mergeCell ref="A3:E3"/>
-    <mergeCell ref="A4:E4"/>
-    <mergeCell ref="F3:H3"/>
     <mergeCell ref="A6:A7"/>
     <mergeCell ref="A2:H2"/>
     <mergeCell ref="A8:H8"/>
@@ -2788,6 +2783,11 @@
     <mergeCell ref="A27:H27"/>
     <mergeCell ref="B6:B7"/>
     <mergeCell ref="A5:H5"/>
+    <mergeCell ref="G1:H1"/>
+    <mergeCell ref="A1:F1"/>
+    <mergeCell ref="A3:E3"/>
+    <mergeCell ref="A4:E4"/>
+    <mergeCell ref="F3:H3"/>
   </mergeCells>
   <phoneticPr fontId="2" type="noConversion"/>
   <printOptions horizontalCentered="1" verticalCentered="1"/>
@@ -2799,15 +2799,6 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
 <p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
   <documentManagement>
     <lcf76f155ced4ddcb4097134ff3c332f xmlns="44fce352-7b49-42d3-bc69-12da48d9ebc0">
@@ -2816,6 +2807,15 @@
     <TaxCatchAll xmlns="fbb90945-3c4c-43b7-bb15-9ae99079c100" xsi:nil="true"/>
   </documentManagement>
 </p:properties>
+</file>
+
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
 </file>
 
 <file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
@@ -3048,14 +3048,6 @@
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{4209C33D-ED08-404F-9B7A-29CD40C2ACA2}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{CD1FC233-9ECF-4A55-86D4-136E16072842}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="44fce352-7b49-42d3-bc69-12da48d9ebc0"/>
@@ -3068,6 +3060,14 @@
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
     <ds:schemaRef ds:uri="fbb90945-3c4c-43b7-bb15-9ae99079c100"/>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{4209C33D-ED08-404F-9B7A-29CD40C2ACA2}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>

</xml_diff>

<commit_message>
Add new documentation files, update styles, and enhance navigation
</commit_message>
<xml_diff>
--- a/assets/synthesegabriel.xlsx
+++ b/assets/synthesegabriel.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://testipformation-my.sharepoint.com/personal/g_martin_ecole-ipssi_net/Documents/IPSSI/Portfolio Final/assets/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="115" documentId="8_{11A09743-F9E9-41CF-B94B-EEA8224A8669}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{A9C8E924-67C5-3645-A5C6-616B7D840A1C}"/>
+  <xr:revisionPtr revIDLastSave="127" documentId="8_{11A09743-F9E9-41CF-B94B-EEA8224A8669}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{C4A9D7FE-0580-2945-92CE-B49796ECD708}"/>
   <bookViews>
     <workbookView showHorizontalScroll="0" showVerticalScroll="0" showSheetTabs="0" xWindow="0" yWindow="900" windowWidth="29400" windowHeight="16980" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -39,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="70" uniqueCount="53">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="74" uniqueCount="53">
   <si>
     <t>BTS SERVICES INFORMATIQUES AUX ORGANISATIONS</t>
   </si>
@@ -156,10 +156,6 @@
     <t>du 01/11/24 au 15/02/24</t>
   </si>
   <si>
-    <t xml:space="preserve">Réalisation de mon Portfolio
-</t>
-  </si>
-  <si>
     <t>Réalisation du site web InfoLab</t>
   </si>
   <si>
@@ -195,9 +191,6 @@
     <t>du 16/09/24 au 23/05/24</t>
   </si>
   <si>
-    <t>du 10/04/23 au 23/05/24</t>
-  </si>
-  <si>
     <t>Centre de formation : IPSSI</t>
   </si>
   <si>
@@ -219,7 +212,14 @@
     <t>09/09/24 au 20/12/24</t>
   </si>
   <si>
-    <t>du 08/01/25 au 23/05/25</t>
+    <t xml:space="preserve">Réalisation d'un Portfolio
+</t>
+  </si>
+  <si>
+    <t>du 06/01/25 au 17/03/25</t>
+  </si>
+  <si>
+    <t>du 10/04/23 au 23/05/25</t>
   </si>
 </sst>
 </file>
@@ -773,9 +773,48 @@
     <xf numFmtId="0" fontId="11" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="27" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="19" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="28" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="20" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
@@ -798,45 +837,6 @@
       <alignment horizontal="left" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="24" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="27" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="19" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="28" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
   </cellXfs>
@@ -1208,8 +1208,8 @@
   </sheetPr>
   <dimension ref="A1:AQ81"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A6" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <selection activeCell="F13" sqref="F13:G14"/>
+    <sheetView tabSelected="1" topLeftCell="A8" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
+      <selection activeCell="H15" sqref="H15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="10.83203125" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
@@ -1222,56 +1222,56 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:43" ht="40" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A1" s="26" t="s">
+      <c r="A1" s="28" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="26"/>
-      <c r="C1" s="26"/>
-      <c r="D1" s="26"/>
-      <c r="E1" s="26"/>
-      <c r="F1" s="26"/>
-      <c r="G1" s="26" t="s">
-        <v>46</v>
-      </c>
-      <c r="H1" s="26"/>
+      <c r="B1" s="28"/>
+      <c r="C1" s="28"/>
+      <c r="D1" s="28"/>
+      <c r="E1" s="28"/>
+      <c r="F1" s="28"/>
+      <c r="G1" s="28" t="s">
+        <v>44</v>
+      </c>
+      <c r="H1" s="28"/>
     </row>
     <row r="2" spans="1:43" ht="41" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A2" s="26" t="s">
+      <c r="A2" s="28" t="s">
         <v>1</v>
       </c>
-      <c r="B2" s="26"/>
-      <c r="C2" s="26"/>
-      <c r="D2" s="26"/>
-      <c r="E2" s="26"/>
-      <c r="F2" s="26"/>
-      <c r="G2" s="26"/>
-      <c r="H2" s="26"/>
+      <c r="B2" s="28"/>
+      <c r="C2" s="28"/>
+      <c r="D2" s="28"/>
+      <c r="E2" s="28"/>
+      <c r="F2" s="28"/>
+      <c r="G2" s="28"/>
+      <c r="H2" s="28"/>
     </row>
     <row r="3" spans="1:43" ht="40" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A3" s="27" t="s">
+      <c r="A3" s="40" t="s">
         <v>23</v>
       </c>
-      <c r="B3" s="28"/>
-      <c r="C3" s="28"/>
-      <c r="D3" s="28"/>
-      <c r="E3" s="29"/>
-      <c r="F3" s="33" t="s">
+      <c r="B3" s="41"/>
+      <c r="C3" s="41"/>
+      <c r="D3" s="41"/>
+      <c r="E3" s="42"/>
+      <c r="F3" s="46" t="s">
         <v>2</v>
       </c>
-      <c r="G3" s="28"/>
-      <c r="H3" s="34"/>
+      <c r="G3" s="41"/>
+      <c r="H3" s="47"/>
       <c r="K3" s="1"/>
       <c r="L3" s="1"/>
       <c r="M3" s="1"/>
     </row>
     <row r="4" spans="1:43" ht="40" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A4" s="30" t="s">
-        <v>45</v>
-      </c>
-      <c r="B4" s="31"/>
-      <c r="C4" s="31"/>
-      <c r="D4" s="31"/>
-      <c r="E4" s="32"/>
+      <c r="A4" s="43" t="s">
+        <v>43</v>
+      </c>
+      <c r="B4" s="44"/>
+      <c r="C4" s="44"/>
+      <c r="D4" s="44"/>
+      <c r="E4" s="45"/>
       <c r="F4" s="12" t="s">
         <v>3</v>
       </c>
@@ -1283,22 +1283,22 @@
       </c>
     </row>
     <row r="5" spans="1:43" ht="40" customHeight="1" thickBot="1" x14ac:dyDescent="0.2">
-      <c r="A5" s="45" t="s">
+      <c r="A5" s="37" t="s">
         <v>24</v>
       </c>
-      <c r="B5" s="46"/>
-      <c r="C5" s="46"/>
-      <c r="D5" s="46"/>
-      <c r="E5" s="46"/>
-      <c r="F5" s="46"/>
-      <c r="G5" s="46"/>
-      <c r="H5" s="47"/>
+      <c r="B5" s="38"/>
+      <c r="C5" s="38"/>
+      <c r="D5" s="38"/>
+      <c r="E5" s="38"/>
+      <c r="F5" s="38"/>
+      <c r="G5" s="38"/>
+      <c r="H5" s="39"/>
     </row>
     <row r="6" spans="1:43" ht="90" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A6" s="35" t="s">
+      <c r="A6" s="26" t="s">
         <v>6</v>
       </c>
-      <c r="B6" s="43" t="s">
+      <c r="B6" s="35" t="s">
         <v>7</v>
       </c>
       <c r="C6" s="6" t="s">
@@ -1321,8 +1321,8 @@
       </c>
     </row>
     <row r="7" spans="1:43" s="2" customFormat="1" ht="325" customHeight="1" thickBot="1" x14ac:dyDescent="0.2">
-      <c r="A7" s="36"/>
-      <c r="B7" s="44"/>
+      <c r="A7" s="27"/>
+      <c r="B7" s="36"/>
       <c r="C7" s="20" t="s">
         <v>14</v>
       </c>
@@ -1378,16 +1378,16 @@
       <c r="AQ7"/>
     </row>
     <row r="8" spans="1:43" s="2" customFormat="1" ht="18" x14ac:dyDescent="0.15">
-      <c r="A8" s="37" t="s">
+      <c r="A8" s="29" t="s">
         <v>20</v>
       </c>
-      <c r="B8" s="38"/>
-      <c r="C8" s="38"/>
-      <c r="D8" s="38"/>
-      <c r="E8" s="38"/>
-      <c r="F8" s="38"/>
-      <c r="G8" s="38"/>
-      <c r="H8" s="39"/>
+      <c r="B8" s="30"/>
+      <c r="C8" s="30"/>
+      <c r="D8" s="30"/>
+      <c r="E8" s="30"/>
+      <c r="F8" s="30"/>
+      <c r="G8" s="30"/>
+      <c r="H8" s="31"/>
       <c r="I8"/>
       <c r="J8"/>
       <c r="K8"/>
@@ -1426,12 +1426,14 @@
     </row>
     <row r="9" spans="1:43" s="2" customFormat="1" ht="40" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A9" s="9" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="B9" s="8" t="s">
         <v>31</v>
       </c>
-      <c r="C9" s="14"/>
+      <c r="C9" s="14" t="s">
+        <v>30</v>
+      </c>
       <c r="D9" s="24"/>
       <c r="E9" s="24" t="s">
         <v>30</v>
@@ -1477,10 +1479,10 @@
     </row>
     <row r="10" spans="1:43" s="2" customFormat="1" ht="40" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A10" s="9" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="B10" s="8" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="C10" s="24" t="s">
         <v>30</v>
@@ -1528,10 +1530,10 @@
     </row>
     <row r="11" spans="1:43" s="2" customFormat="1" ht="40" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A11" s="9" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="B11" s="8" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="C11" s="15"/>
       <c r="D11" s="15"/>
@@ -1579,10 +1581,10 @@
     </row>
     <row r="12" spans="1:43" s="2" customFormat="1" ht="40" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A12" s="9" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="B12" s="8" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="C12" s="24" t="s">
         <v>30</v>
@@ -1634,12 +1636,14 @@
     </row>
     <row r="13" spans="1:43" s="2" customFormat="1" ht="40" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A13" s="9" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="B13" s="8" t="s">
-        <v>43</v>
-      </c>
-      <c r="C13" s="15"/>
+        <v>42</v>
+      </c>
+      <c r="C13" s="24" t="s">
+        <v>30</v>
+      </c>
       <c r="D13" s="15"/>
       <c r="E13" s="15"/>
       <c r="F13" s="24" t="s">
@@ -1687,12 +1691,14 @@
     </row>
     <row r="14" spans="1:43" s="2" customFormat="1" ht="40" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A14" s="9" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="B14" s="8" t="s">
-        <v>52</v>
-      </c>
-      <c r="C14" s="15"/>
+        <v>51</v>
+      </c>
+      <c r="C14" s="24" t="s">
+        <v>30</v>
+      </c>
       <c r="D14" s="15"/>
       <c r="E14" s="15"/>
       <c r="F14" s="24" t="s">
@@ -1740,10 +1746,10 @@
     </row>
     <row r="15" spans="1:43" s="2" customFormat="1" ht="40" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A15" s="9" t="s">
-        <v>32</v>
+        <v>50</v>
       </c>
       <c r="B15" s="8" t="s">
-        <v>44</v>
+        <v>52</v>
       </c>
       <c r="C15" s="15"/>
       <c r="D15" s="15"/>
@@ -1924,16 +1930,16 @@
       <c r="AQ18"/>
     </row>
     <row r="19" spans="1:43" s="2" customFormat="1" ht="18" x14ac:dyDescent="0.15">
-      <c r="A19" s="40" t="s">
+      <c r="A19" s="32" t="s">
         <v>21</v>
       </c>
-      <c r="B19" s="41"/>
-      <c r="C19" s="41"/>
-      <c r="D19" s="41"/>
-      <c r="E19" s="41"/>
-      <c r="F19" s="41"/>
-      <c r="G19" s="41"/>
-      <c r="H19" s="42"/>
+      <c r="B19" s="33"/>
+      <c r="C19" s="33"/>
+      <c r="D19" s="33"/>
+      <c r="E19" s="33"/>
+      <c r="F19" s="33"/>
+      <c r="G19" s="33"/>
+      <c r="H19" s="34"/>
       <c r="I19"/>
       <c r="J19"/>
       <c r="K19"/>
@@ -1975,7 +1981,7 @@
         <v>25</v>
       </c>
       <c r="B20" s="22" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
       <c r="C20" s="15"/>
       <c r="D20" s="15"/>
@@ -2304,16 +2310,16 @@
       <c r="AQ26"/>
     </row>
     <row r="27" spans="1:43" s="2" customFormat="1" ht="18" x14ac:dyDescent="0.15">
-      <c r="A27" s="40" t="s">
+      <c r="A27" s="32" t="s">
         <v>22</v>
       </c>
-      <c r="B27" s="41"/>
-      <c r="C27" s="41"/>
-      <c r="D27" s="41"/>
-      <c r="E27" s="41"/>
-      <c r="F27" s="41"/>
-      <c r="G27" s="41"/>
-      <c r="H27" s="42"/>
+      <c r="B27" s="33"/>
+      <c r="C27" s="33"/>
+      <c r="D27" s="33"/>
+      <c r="E27" s="33"/>
+      <c r="F27" s="33"/>
+      <c r="G27" s="33"/>
+      <c r="H27" s="34"/>
       <c r="I27"/>
       <c r="J27"/>
       <c r="K27"/>
@@ -2352,10 +2358,10 @@
     </row>
     <row r="28" spans="1:43" s="2" customFormat="1" ht="40" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A28" s="9" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="B28" s="8" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
       <c r="C28" s="15"/>
       <c r="D28" s="15"/>
@@ -2406,7 +2412,7 @@
         <v>27</v>
       </c>
       <c r="B29" s="8" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
       <c r="C29" s="15"/>
       <c r="D29" s="15"/>
@@ -2454,13 +2460,15 @@
     </row>
     <row r="30" spans="1:43" s="2" customFormat="1" ht="40" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A30" s="9" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
       <c r="B30" s="8" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
       <c r="C30" s="15"/>
-      <c r="D30" s="15"/>
+      <c r="D30" s="24" t="s">
+        <v>30</v>
+      </c>
       <c r="E30" s="15"/>
       <c r="F30" s="24" t="s">
         <v>30</v>
@@ -2776,6 +2784,11 @@
     <row r="81" customFormat="1" x14ac:dyDescent="0.15"/>
   </sheetData>
   <mergeCells count="12">
+    <mergeCell ref="G1:H1"/>
+    <mergeCell ref="A1:F1"/>
+    <mergeCell ref="A3:E3"/>
+    <mergeCell ref="A4:E4"/>
+    <mergeCell ref="F3:H3"/>
     <mergeCell ref="A6:A7"/>
     <mergeCell ref="A2:H2"/>
     <mergeCell ref="A8:H8"/>
@@ -2783,11 +2796,6 @@
     <mergeCell ref="A27:H27"/>
     <mergeCell ref="B6:B7"/>
     <mergeCell ref="A5:H5"/>
-    <mergeCell ref="G1:H1"/>
-    <mergeCell ref="A1:F1"/>
-    <mergeCell ref="A3:E3"/>
-    <mergeCell ref="A4:E4"/>
-    <mergeCell ref="F3:H3"/>
   </mergeCells>
   <phoneticPr fontId="2" type="noConversion"/>
   <printOptions horizontalCentered="1" verticalCentered="1"/>
@@ -2810,15 +2818,6 @@
 </file>
 
 <file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x010100B44D25FE6749554FA89155DE40CE9E1E" ma:contentTypeVersion="14" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="8bb8039247b655a9c70bf36b5dd9dc64">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="44fce352-7b49-42d3-bc69-12da48d9ebc0" xmlns:ns3="fbb90945-3c4c-43b7-bb15-9ae99079c100" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="85d91c69c6e00024127dca24cda9fdf4" ns2:_="" ns3:_="">
     <xsd:import namespace="44fce352-7b49-42d3-bc69-12da48d9ebc0"/>
@@ -3047,32 +3046,33 @@
 </ct:contentTypeSchema>
 </file>
 
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{CD1FC233-9ECF-4A55-86D4-136E16072842}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="44fce352-7b49-42d3-bc69-12da48d9ebc0"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
     <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
-    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
     <ds:schemaRef ds:uri="fbb90945-3c4c-43b7-bb15-9ae99079c100"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="44fce352-7b49-42d3-bc69-12da48d9ebc0"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
 
 <file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{4209C33D-ED08-404F-9B7A-29CD40C2ACA2}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{36ECBC65-C27A-4C6D-BAE3-04A998F6FAE4}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -3089,4 +3089,12 @@
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{4209C33D-ED08-404F-9B7A-29CD40C2ACA2}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
</xml_diff>

<commit_message>
Add new assets and improve styling for better layout and spacing
</commit_message>
<xml_diff>
--- a/assets/synthesegabriel.xlsx
+++ b/assets/synthesegabriel.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://testipformation-my.sharepoint.com/personal/g_martin_ecole-ipssi_net/Documents/IPSSI/Portfolio Final/assets/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="127" documentId="8_{11A09743-F9E9-41CF-B94B-EEA8224A8669}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{C4A9D7FE-0580-2945-92CE-B49796ECD708}"/>
+  <xr:revisionPtr revIDLastSave="1" documentId="14_{7489D02B-8F26-2240-870B-C93D8F98F8A1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{5468858D-5B99-7846-A510-2099F9D65396}"/>
   <bookViews>
-    <workbookView showHorizontalScroll="0" showVerticalScroll="0" showSheetTabs="0" xWindow="0" yWindow="900" windowWidth="29400" windowHeight="16980" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView showHorizontalScroll="0" showVerticalScroll="0" showSheetTabs="0" xWindow="0" yWindow="860" windowWidth="29400" windowHeight="16980" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Tableau de synthèse Épreuve E4" sheetId="1" r:id="rId1"/>
@@ -39,15 +39,12 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="74" uniqueCount="53">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="78" uniqueCount="55">
   <si>
     <t>BTS SERVICES INFORMATIQUES AUX ORGANISATIONS</t>
   </si>
   <si>
     <t xml:space="preserve">Tableau de synthèse des réalisations professionnelles </t>
-  </si>
-  <si>
-    <t xml:space="preserve">N° candidat : </t>
   </si>
   <si>
     <t>Option :</t>
@@ -220,6 +217,15 @@
   </si>
   <si>
     <t>du 10/04/23 au 23/05/25</t>
+  </si>
+  <si>
+    <t>N° candidat : 2444882300</t>
+  </si>
+  <si>
+    <t>Résolution de tickets applicatifs</t>
+  </si>
+  <si>
+    <t>08/01/25 au 22/07/25</t>
   </si>
 </sst>
 </file>
@@ -287,12 +293,12 @@
       <family val="2"/>
     </font>
     <font>
-      <sz val="16"/>
+      <sz val="20"/>
       <name val="Arial"/>
       <family val="2"/>
     </font>
     <font>
-      <sz val="20"/>
+      <sz val="18"/>
       <name val="Arial"/>
       <family val="2"/>
     </font>
@@ -737,41 +743,68 @@
     <xf numFmtId="0" fontId="6" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="26" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1"/>
+    </xf>
+    <xf numFmtId="14" fontId="4" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="10" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="26" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1"/>
-    </xf>
-    <xf numFmtId="14" fontId="4" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="11" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="20" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="21" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="22" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="25" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="23" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="24" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -779,9 +812,6 @@
     <xf numFmtId="0" fontId="5" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -813,30 +843,6 @@
       <alignment horizontal="left" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="28" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="20" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="21" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="22" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="25" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="23" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="24" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
   </cellXfs>
@@ -891,6 +897,7 @@
         <a:prstGeom prst="line">
           <a:avLst/>
         </a:prstGeom>
+        <a:ln w="38100"/>
       </xdr:spPr>
       <xdr:style>
         <a:lnRef idx="1">
@@ -910,10 +917,6 @@
     <xdr:clientData/>
   </xdr:twoCellAnchor>
 </xdr:wsDr>
-</file>
-
-<file path=xl/persons/person.xml><?xml version="1.0" encoding="utf-8"?>
-<personList xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main"/>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -1208,8 +1211,8 @@
   </sheetPr>
   <dimension ref="A1:AQ81"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A8" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <selection activeCell="H15" sqref="H15"/>
+    <sheetView tabSelected="1" topLeftCell="A17" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
+      <selection activeCell="A33" sqref="A33"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="10.83203125" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
@@ -1222,124 +1225,124 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:43" ht="40" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A1" s="28" t="s">
+      <c r="A1" s="26" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="28"/>
-      <c r="C1" s="28"/>
-      <c r="D1" s="28"/>
-      <c r="E1" s="28"/>
-      <c r="F1" s="28"/>
-      <c r="G1" s="28" t="s">
-        <v>44</v>
-      </c>
-      <c r="H1" s="28"/>
+      <c r="B1" s="26"/>
+      <c r="C1" s="26"/>
+      <c r="D1" s="26"/>
+      <c r="E1" s="26"/>
+      <c r="F1" s="26"/>
+      <c r="G1" s="26" t="s">
+        <v>43</v>
+      </c>
+      <c r="H1" s="26"/>
     </row>
     <row r="2" spans="1:43" ht="41" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A2" s="28" t="s">
+      <c r="A2" s="26" t="s">
         <v>1</v>
       </c>
-      <c r="B2" s="28"/>
-      <c r="C2" s="28"/>
-      <c r="D2" s="28"/>
-      <c r="E2" s="28"/>
-      <c r="F2" s="28"/>
-      <c r="G2" s="28"/>
-      <c r="H2" s="28"/>
+      <c r="B2" s="26"/>
+      <c r="C2" s="26"/>
+      <c r="D2" s="26"/>
+      <c r="E2" s="26"/>
+      <c r="F2" s="26"/>
+      <c r="G2" s="26"/>
+      <c r="H2" s="26"/>
     </row>
     <row r="3" spans="1:43" ht="40" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A3" s="40" t="s">
-        <v>23</v>
-      </c>
-      <c r="B3" s="41"/>
-      <c r="C3" s="41"/>
-      <c r="D3" s="41"/>
-      <c r="E3" s="42"/>
-      <c r="F3" s="46" t="s">
-        <v>2</v>
-      </c>
-      <c r="G3" s="41"/>
-      <c r="H3" s="47"/>
+      <c r="A3" s="27" t="s">
+        <v>22</v>
+      </c>
+      <c r="B3" s="28"/>
+      <c r="C3" s="28"/>
+      <c r="D3" s="28"/>
+      <c r="E3" s="29"/>
+      <c r="F3" s="33" t="s">
+        <v>52</v>
+      </c>
+      <c r="G3" s="28"/>
+      <c r="H3" s="34"/>
       <c r="K3" s="1"/>
       <c r="L3" s="1"/>
       <c r="M3" s="1"/>
     </row>
     <row r="4" spans="1:43" ht="40" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A4" s="43" t="s">
-        <v>43</v>
-      </c>
-      <c r="B4" s="44"/>
-      <c r="C4" s="44"/>
-      <c r="D4" s="44"/>
-      <c r="E4" s="45"/>
+      <c r="A4" s="30" t="s">
+        <v>42</v>
+      </c>
+      <c r="B4" s="31"/>
+      <c r="C4" s="31"/>
+      <c r="D4" s="31"/>
+      <c r="E4" s="32"/>
       <c r="F4" s="12" t="s">
+        <v>2</v>
+      </c>
+      <c r="G4" s="13" t="s">
         <v>3</v>
       </c>
-      <c r="G4" s="13" t="s">
+      <c r="H4" s="18" t="s">
         <v>4</v>
       </c>
-      <c r="H4" s="19" t="s">
+    </row>
+    <row r="5" spans="1:43" ht="40" customHeight="1" thickBot="1" x14ac:dyDescent="0.2">
+      <c r="A5" s="45" t="s">
+        <v>23</v>
+      </c>
+      <c r="B5" s="46"/>
+      <c r="C5" s="46"/>
+      <c r="D5" s="46"/>
+      <c r="E5" s="46"/>
+      <c r="F5" s="46"/>
+      <c r="G5" s="46"/>
+      <c r="H5" s="47"/>
+    </row>
+    <row r="6" spans="1:43" ht="90" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A6" s="35" t="s">
         <v>5</v>
       </c>
-    </row>
-    <row r="5" spans="1:43" ht="40" customHeight="1" thickBot="1" x14ac:dyDescent="0.2">
-      <c r="A5" s="37" t="s">
-        <v>24</v>
-      </c>
-      <c r="B5" s="38"/>
-      <c r="C5" s="38"/>
-      <c r="D5" s="38"/>
-      <c r="E5" s="38"/>
-      <c r="F5" s="38"/>
-      <c r="G5" s="38"/>
-      <c r="H5" s="39"/>
-    </row>
-    <row r="6" spans="1:43" ht="90" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A6" s="26" t="s">
+      <c r="B6" s="43" t="s">
         <v>6</v>
       </c>
-      <c r="B6" s="35" t="s">
+      <c r="C6" s="6" t="s">
         <v>7</v>
       </c>
-      <c r="C6" s="6" t="s">
+      <c r="D6" s="6" t="s">
         <v>8</v>
       </c>
-      <c r="D6" s="6" t="s">
+      <c r="E6" s="6" t="s">
         <v>9</v>
       </c>
-      <c r="E6" s="6" t="s">
+      <c r="F6" s="6" t="s">
         <v>10</v>
       </c>
-      <c r="F6" s="6" t="s">
+      <c r="G6" s="6" t="s">
         <v>11</v>
       </c>
-      <c r="G6" s="6" t="s">
+      <c r="H6" s="7" t="s">
         <v>12</v>
       </c>
-      <c r="H6" s="7" t="s">
+    </row>
+    <row r="7" spans="1:43" s="2" customFormat="1" ht="325" customHeight="1" thickBot="1" x14ac:dyDescent="0.2">
+      <c r="A7" s="36"/>
+      <c r="B7" s="44"/>
+      <c r="C7" s="19" t="s">
         <v>13</v>
       </c>
-    </row>
-    <row r="7" spans="1:43" s="2" customFormat="1" ht="325" customHeight="1" thickBot="1" x14ac:dyDescent="0.2">
-      <c r="A7" s="27"/>
-      <c r="B7" s="36"/>
-      <c r="C7" s="20" t="s">
+      <c r="D7" s="19" t="s">
         <v>14</v>
       </c>
-      <c r="D7" s="20" t="s">
+      <c r="E7" s="19" t="s">
         <v>15</v>
       </c>
-      <c r="E7" s="20" t="s">
+      <c r="F7" s="19" t="s">
         <v>16</v>
       </c>
-      <c r="F7" s="20" t="s">
+      <c r="G7" s="19" t="s">
         <v>17</v>
       </c>
-      <c r="G7" s="20" t="s">
+      <c r="H7" s="20" t="s">
         <v>18</v>
-      </c>
-      <c r="H7" s="21" t="s">
-        <v>19</v>
       </c>
       <c r="I7"/>
       <c r="J7"/>
@@ -1378,16 +1381,16 @@
       <c r="AQ7"/>
     </row>
     <row r="8" spans="1:43" s="2" customFormat="1" ht="18" x14ac:dyDescent="0.15">
-      <c r="A8" s="29" t="s">
-        <v>20</v>
-      </c>
-      <c r="B8" s="30"/>
-      <c r="C8" s="30"/>
-      <c r="D8" s="30"/>
-      <c r="E8" s="30"/>
-      <c r="F8" s="30"/>
-      <c r="G8" s="30"/>
-      <c r="H8" s="31"/>
+      <c r="A8" s="37" t="s">
+        <v>19</v>
+      </c>
+      <c r="B8" s="38"/>
+      <c r="C8" s="38"/>
+      <c r="D8" s="38"/>
+      <c r="E8" s="38"/>
+      <c r="F8" s="38"/>
+      <c r="G8" s="38"/>
+      <c r="H8" s="39"/>
       <c r="I8"/>
       <c r="J8"/>
       <c r="K8"/>
@@ -1426,21 +1429,21 @@
     </row>
     <row r="9" spans="1:43" s="2" customFormat="1" ht="40" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A9" s="9" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="B9" s="8" t="s">
-        <v>31</v>
-      </c>
-      <c r="C9" s="14" t="s">
         <v>30</v>
       </c>
-      <c r="D9" s="24"/>
-      <c r="E9" s="24" t="s">
-        <v>30</v>
-      </c>
-      <c r="F9" s="15"/>
-      <c r="G9" s="15"/>
-      <c r="H9" s="23"/>
+      <c r="C9" s="25" t="s">
+        <v>29</v>
+      </c>
+      <c r="D9" s="23"/>
+      <c r="E9" s="23" t="s">
+        <v>29</v>
+      </c>
+      <c r="F9" s="14"/>
+      <c r="G9" s="14"/>
+      <c r="H9" s="22"/>
       <c r="I9"/>
       <c r="J9"/>
       <c r="K9"/>
@@ -1479,19 +1482,19 @@
     </row>
     <row r="10" spans="1:43" s="2" customFormat="1" ht="40" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A10" s="9" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="B10" s="8" t="s">
-        <v>39</v>
-      </c>
-      <c r="C10" s="24" t="s">
-        <v>30</v>
-      </c>
-      <c r="D10" s="15"/>
-      <c r="E10" s="15"/>
-      <c r="F10" s="15"/>
-      <c r="G10" s="15"/>
-      <c r="H10" s="23"/>
+        <v>38</v>
+      </c>
+      <c r="C10" s="23" t="s">
+        <v>29</v>
+      </c>
+      <c r="D10" s="14"/>
+      <c r="E10" s="14"/>
+      <c r="F10" s="14"/>
+      <c r="G10" s="14"/>
+      <c r="H10" s="22"/>
       <c r="I10"/>
       <c r="J10"/>
       <c r="K10"/>
@@ -1530,18 +1533,18 @@
     </row>
     <row r="11" spans="1:43" s="2" customFormat="1" ht="40" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A11" s="9" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="B11" s="8" t="s">
-        <v>40</v>
-      </c>
-      <c r="C11" s="15"/>
-      <c r="D11" s="15"/>
-      <c r="E11" s="15"/>
-      <c r="F11" s="15"/>
-      <c r="G11" s="15"/>
-      <c r="H11" s="23" t="s">
-        <v>30</v>
+        <v>39</v>
+      </c>
+      <c r="C11" s="14"/>
+      <c r="D11" s="14"/>
+      <c r="E11" s="14"/>
+      <c r="F11" s="14"/>
+      <c r="G11" s="14"/>
+      <c r="H11" s="22" t="s">
+        <v>29</v>
       </c>
       <c r="I11"/>
       <c r="J11"/>
@@ -1581,23 +1584,23 @@
     </row>
     <row r="12" spans="1:43" s="2" customFormat="1" ht="40" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A12" s="9" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="B12" s="8" t="s">
-        <v>41</v>
-      </c>
-      <c r="C12" s="24" t="s">
-        <v>30</v>
-      </c>
-      <c r="D12" s="24" t="s">
-        <v>30</v>
-      </c>
-      <c r="E12" s="15"/>
-      <c r="F12" s="24"/>
-      <c r="G12" s="24" t="s">
-        <v>30</v>
-      </c>
-      <c r="H12" s="16"/>
+        <v>40</v>
+      </c>
+      <c r="C12" s="23" t="s">
+        <v>29</v>
+      </c>
+      <c r="D12" s="23" t="s">
+        <v>29</v>
+      </c>
+      <c r="E12" s="14"/>
+      <c r="F12" s="23"/>
+      <c r="G12" s="23" t="s">
+        <v>29</v>
+      </c>
+      <c r="H12" s="15"/>
       <c r="I12"/>
       <c r="J12"/>
       <c r="K12"/>
@@ -1636,23 +1639,23 @@
     </row>
     <row r="13" spans="1:43" s="2" customFormat="1" ht="40" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A13" s="9" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="B13" s="8" t="s">
-        <v>42</v>
-      </c>
-      <c r="C13" s="24" t="s">
-        <v>30</v>
-      </c>
-      <c r="D13" s="15"/>
-      <c r="E13" s="15"/>
-      <c r="F13" s="24" t="s">
-        <v>30</v>
-      </c>
-      <c r="G13" s="25" t="s">
-        <v>30</v>
-      </c>
-      <c r="H13" s="23"/>
+        <v>41</v>
+      </c>
+      <c r="C13" s="23" t="s">
+        <v>29</v>
+      </c>
+      <c r="D13" s="14"/>
+      <c r="E13" s="14"/>
+      <c r="F13" s="23" t="s">
+        <v>29</v>
+      </c>
+      <c r="G13" s="24" t="s">
+        <v>29</v>
+      </c>
+      <c r="H13" s="22"/>
       <c r="I13"/>
       <c r="J13"/>
       <c r="K13"/>
@@ -1691,23 +1694,23 @@
     </row>
     <row r="14" spans="1:43" s="2" customFormat="1" ht="40" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A14" s="9" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="B14" s="8" t="s">
-        <v>51</v>
-      </c>
-      <c r="C14" s="24" t="s">
-        <v>30</v>
-      </c>
-      <c r="D14" s="15"/>
-      <c r="E14" s="15"/>
-      <c r="F14" s="24" t="s">
-        <v>30</v>
-      </c>
-      <c r="G14" s="24" t="s">
-        <v>30</v>
-      </c>
-      <c r="H14" s="23"/>
+        <v>50</v>
+      </c>
+      <c r="C14" s="23" t="s">
+        <v>29</v>
+      </c>
+      <c r="D14" s="14"/>
+      <c r="E14" s="14"/>
+      <c r="F14" s="23" t="s">
+        <v>29</v>
+      </c>
+      <c r="G14" s="23" t="s">
+        <v>29</v>
+      </c>
+      <c r="H14" s="22"/>
       <c r="I14"/>
       <c r="J14"/>
       <c r="K14"/>
@@ -1746,18 +1749,18 @@
     </row>
     <row r="15" spans="1:43" s="2" customFormat="1" ht="40" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A15" s="9" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="B15" s="8" t="s">
-        <v>52</v>
-      </c>
-      <c r="C15" s="15"/>
-      <c r="D15" s="15"/>
-      <c r="E15" s="15"/>
-      <c r="F15" s="15"/>
-      <c r="G15" s="15"/>
-      <c r="H15" s="23" t="s">
-        <v>30</v>
+        <v>51</v>
+      </c>
+      <c r="C15" s="14"/>
+      <c r="D15" s="14"/>
+      <c r="E15" s="14"/>
+      <c r="F15" s="14"/>
+      <c r="G15" s="14"/>
+      <c r="H15" s="22" t="s">
+        <v>29</v>
       </c>
       <c r="I15"/>
       <c r="J15"/>
@@ -1798,12 +1801,12 @@
     <row r="16" spans="1:43" s="2" customFormat="1" ht="40" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A16" s="9"/>
       <c r="B16" s="8"/>
-      <c r="C16" s="15"/>
-      <c r="D16" s="15"/>
-      <c r="E16" s="24"/>
-      <c r="F16" s="15"/>
-      <c r="G16" s="15"/>
-      <c r="H16" s="16"/>
+      <c r="C16" s="14"/>
+      <c r="D16" s="14"/>
+      <c r="E16" s="23"/>
+      <c r="F16" s="14"/>
+      <c r="G16" s="14"/>
+      <c r="H16" s="15"/>
       <c r="I16"/>
       <c r="J16"/>
       <c r="K16"/>
@@ -1843,11 +1846,11 @@
     <row r="17" spans="1:43" s="2" customFormat="1" ht="40" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A17" s="9"/>
       <c r="B17" s="8"/>
-      <c r="C17" s="15"/>
-      <c r="D17" s="15"/>
-      <c r="F17" s="15"/>
-      <c r="G17" s="15"/>
-      <c r="H17" s="16"/>
+      <c r="C17" s="14"/>
+      <c r="D17" s="14"/>
+      <c r="F17" s="14"/>
+      <c r="G17" s="14"/>
+      <c r="H17" s="15"/>
       <c r="I17"/>
       <c r="J17"/>
       <c r="K17"/>
@@ -1887,12 +1890,12 @@
     <row r="18" spans="1:43" s="2" customFormat="1" ht="40" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A18" s="9"/>
       <c r="B18" s="8"/>
-      <c r="C18" s="15"/>
-      <c r="D18" s="15"/>
-      <c r="E18" s="15"/>
-      <c r="F18" s="15"/>
-      <c r="G18" s="15"/>
-      <c r="H18" s="16"/>
+      <c r="C18" s="14"/>
+      <c r="D18" s="14"/>
+      <c r="E18" s="14"/>
+      <c r="F18" s="14"/>
+      <c r="G18" s="14"/>
+      <c r="H18" s="15"/>
       <c r="I18"/>
       <c r="J18"/>
       <c r="K18"/>
@@ -1930,16 +1933,16 @@
       <c r="AQ18"/>
     </row>
     <row r="19" spans="1:43" s="2" customFormat="1" ht="18" x14ac:dyDescent="0.15">
-      <c r="A19" s="32" t="s">
-        <v>21</v>
-      </c>
-      <c r="B19" s="33"/>
-      <c r="C19" s="33"/>
-      <c r="D19" s="33"/>
-      <c r="E19" s="33"/>
-      <c r="F19" s="33"/>
-      <c r="G19" s="33"/>
-      <c r="H19" s="34"/>
+      <c r="A19" s="40" t="s">
+        <v>20</v>
+      </c>
+      <c r="B19" s="41"/>
+      <c r="C19" s="41"/>
+      <c r="D19" s="41"/>
+      <c r="E19" s="41"/>
+      <c r="F19" s="41"/>
+      <c r="G19" s="41"/>
+      <c r="H19" s="42"/>
       <c r="I19"/>
       <c r="J19"/>
       <c r="K19"/>
@@ -1978,19 +1981,19 @@
     </row>
     <row r="20" spans="1:43" s="2" customFormat="1" ht="40" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A20" s="9" t="s">
-        <v>25</v>
-      </c>
-      <c r="B20" s="22" t="s">
-        <v>47</v>
-      </c>
-      <c r="C20" s="15"/>
-      <c r="D20" s="15"/>
-      <c r="E20" s="15"/>
-      <c r="F20" s="15"/>
-      <c r="G20" s="24" t="s">
-        <v>30</v>
-      </c>
-      <c r="H20" s="16"/>
+        <v>24</v>
+      </c>
+      <c r="B20" s="21" t="s">
+        <v>46</v>
+      </c>
+      <c r="C20" s="14"/>
+      <c r="D20" s="14"/>
+      <c r="E20" s="14"/>
+      <c r="F20" s="14"/>
+      <c r="G20" s="23" t="s">
+        <v>29</v>
+      </c>
+      <c r="H20" s="15"/>
       <c r="I20"/>
       <c r="J20"/>
       <c r="K20"/>
@@ -2029,19 +2032,19 @@
     </row>
     <row r="21" spans="1:43" s="2" customFormat="1" ht="40" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A21" s="9" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="B21" s="8" t="s">
-        <v>28</v>
-      </c>
-      <c r="C21" s="15"/>
-      <c r="D21" s="15"/>
-      <c r="E21" s="15"/>
-      <c r="F21" s="15"/>
-      <c r="G21" s="24" t="s">
-        <v>30</v>
-      </c>
-      <c r="H21" s="16"/>
+        <v>27</v>
+      </c>
+      <c r="C21" s="14"/>
+      <c r="D21" s="14"/>
+      <c r="E21" s="14"/>
+      <c r="F21" s="14"/>
+      <c r="G21" s="23" t="s">
+        <v>29</v>
+      </c>
+      <c r="H21" s="15"/>
       <c r="I21"/>
       <c r="J21"/>
       <c r="K21"/>
@@ -2080,19 +2083,19 @@
     </row>
     <row r="22" spans="1:43" s="2" customFormat="1" ht="40" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A22" s="9" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="B22" s="8" t="s">
+        <v>28</v>
+      </c>
+      <c r="C22" s="14"/>
+      <c r="D22" s="14"/>
+      <c r="E22" s="23" t="s">
         <v>29</v>
       </c>
-      <c r="C22" s="15"/>
-      <c r="D22" s="15"/>
-      <c r="E22" s="24" t="s">
-        <v>30</v>
-      </c>
-      <c r="F22" s="15"/>
-      <c r="G22" s="15"/>
-      <c r="H22" s="16"/>
+      <c r="F22" s="14"/>
+      <c r="G22" s="14"/>
+      <c r="H22" s="15"/>
       <c r="I22"/>
       <c r="J22"/>
       <c r="K22"/>
@@ -2132,12 +2135,12 @@
     <row r="23" spans="1:43" s="2" customFormat="1" ht="40" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A23" s="9"/>
       <c r="B23" s="8"/>
-      <c r="C23" s="15"/>
-      <c r="D23" s="15"/>
-      <c r="E23" s="15"/>
-      <c r="F23" s="15"/>
-      <c r="G23" s="15"/>
-      <c r="H23" s="16"/>
+      <c r="C23" s="14"/>
+      <c r="D23" s="14"/>
+      <c r="E23" s="14"/>
+      <c r="F23" s="14"/>
+      <c r="G23" s="14"/>
+      <c r="H23" s="15"/>
       <c r="I23"/>
       <c r="J23"/>
       <c r="K23"/>
@@ -2177,12 +2180,12 @@
     <row r="24" spans="1:43" s="2" customFormat="1" ht="40" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A24" s="9"/>
       <c r="B24" s="8"/>
-      <c r="C24" s="15"/>
-      <c r="D24" s="15"/>
-      <c r="E24" s="15"/>
-      <c r="F24" s="15"/>
-      <c r="G24" s="15"/>
-      <c r="H24" s="16"/>
+      <c r="C24" s="14"/>
+      <c r="D24" s="14"/>
+      <c r="E24" s="14"/>
+      <c r="F24" s="14"/>
+      <c r="G24" s="14"/>
+      <c r="H24" s="15"/>
       <c r="I24"/>
       <c r="J24"/>
       <c r="K24"/>
@@ -2222,12 +2225,12 @@
     <row r="25" spans="1:43" s="2" customFormat="1" ht="40" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A25" s="9"/>
       <c r="B25" s="8"/>
-      <c r="C25" s="15"/>
-      <c r="D25" s="15"/>
-      <c r="E25" s="15"/>
-      <c r="F25" s="15"/>
-      <c r="G25" s="15"/>
-      <c r="H25" s="16"/>
+      <c r="C25" s="14"/>
+      <c r="D25" s="14"/>
+      <c r="E25" s="14"/>
+      <c r="F25" s="14"/>
+      <c r="G25" s="14"/>
+      <c r="H25" s="15"/>
       <c r="I25"/>
       <c r="J25"/>
       <c r="K25"/>
@@ -2267,12 +2270,12 @@
     <row r="26" spans="1:43" s="2" customFormat="1" ht="40" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A26" s="9"/>
       <c r="B26" s="8"/>
-      <c r="C26" s="15"/>
-      <c r="D26" s="15"/>
-      <c r="E26" s="15"/>
-      <c r="F26" s="15"/>
-      <c r="G26" s="15"/>
-      <c r="H26" s="16"/>
+      <c r="C26" s="14"/>
+      <c r="D26" s="14"/>
+      <c r="E26" s="14"/>
+      <c r="F26" s="14"/>
+      <c r="G26" s="14"/>
+      <c r="H26" s="15"/>
       <c r="I26"/>
       <c r="J26"/>
       <c r="K26"/>
@@ -2310,16 +2313,16 @@
       <c r="AQ26"/>
     </row>
     <row r="27" spans="1:43" s="2" customFormat="1" ht="18" x14ac:dyDescent="0.15">
-      <c r="A27" s="32" t="s">
-        <v>22</v>
-      </c>
-      <c r="B27" s="33"/>
-      <c r="C27" s="33"/>
-      <c r="D27" s="33"/>
-      <c r="E27" s="33"/>
-      <c r="F27" s="33"/>
-      <c r="G27" s="33"/>
-      <c r="H27" s="34"/>
+      <c r="A27" s="40" t="s">
+        <v>21</v>
+      </c>
+      <c r="B27" s="41"/>
+      <c r="C27" s="41"/>
+      <c r="D27" s="41"/>
+      <c r="E27" s="41"/>
+      <c r="F27" s="41"/>
+      <c r="G27" s="41"/>
+      <c r="H27" s="42"/>
       <c r="I27"/>
       <c r="J27"/>
       <c r="K27"/>
@@ -2358,19 +2361,19 @@
     </row>
     <row r="28" spans="1:43" s="2" customFormat="1" ht="40" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A28" s="9" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="B28" s="8" t="s">
-        <v>46</v>
-      </c>
-      <c r="C28" s="15"/>
-      <c r="D28" s="15"/>
-      <c r="E28" s="24" t="s">
-        <v>30</v>
-      </c>
-      <c r="F28" s="15"/>
-      <c r="G28" s="15"/>
-      <c r="H28" s="16"/>
+        <v>45</v>
+      </c>
+      <c r="C28" s="14"/>
+      <c r="D28" s="14"/>
+      <c r="E28" s="23" t="s">
+        <v>29</v>
+      </c>
+      <c r="F28" s="14"/>
+      <c r="G28" s="14"/>
+      <c r="H28" s="15"/>
       <c r="I28"/>
       <c r="J28"/>
       <c r="K28"/>
@@ -2409,19 +2412,19 @@
     </row>
     <row r="29" spans="1:43" s="2" customFormat="1" ht="40" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A29" s="9" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="B29" s="8" t="s">
-        <v>49</v>
-      </c>
-      <c r="C29" s="15"/>
-      <c r="D29" s="15"/>
-      <c r="E29" s="24" t="s">
-        <v>30</v>
-      </c>
-      <c r="F29" s="15"/>
-      <c r="G29" s="15"/>
-      <c r="H29" s="16"/>
+        <v>48</v>
+      </c>
+      <c r="C29" s="14"/>
+      <c r="D29" s="14"/>
+      <c r="E29" s="23" t="s">
+        <v>29</v>
+      </c>
+      <c r="F29" s="14"/>
+      <c r="G29" s="14"/>
+      <c r="H29" s="15"/>
       <c r="I29"/>
       <c r="J29"/>
       <c r="K29"/>
@@ -2460,21 +2463,21 @@
     </row>
     <row r="30" spans="1:43" s="2" customFormat="1" ht="40" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A30" s="9" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="B30" s="8" t="s">
-        <v>48</v>
-      </c>
-      <c r="C30" s="15"/>
-      <c r="D30" s="24" t="s">
-        <v>30</v>
-      </c>
-      <c r="E30" s="15"/>
-      <c r="F30" s="24" t="s">
-        <v>30</v>
-      </c>
-      <c r="G30" s="15"/>
-      <c r="H30" s="16"/>
+        <v>47</v>
+      </c>
+      <c r="C30" s="14"/>
+      <c r="D30" s="23" t="s">
+        <v>29</v>
+      </c>
+      <c r="E30" s="14"/>
+      <c r="F30" s="23" t="s">
+        <v>29</v>
+      </c>
+      <c r="G30" s="14"/>
+      <c r="H30" s="15"/>
       <c r="I30"/>
       <c r="J30"/>
       <c r="K30"/>
@@ -2512,14 +2515,22 @@
       <c r="AQ30"/>
     </row>
     <row r="31" spans="1:43" s="2" customFormat="1" ht="40" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A31" s="9"/>
-      <c r="B31" s="8"/>
-      <c r="C31" s="15"/>
-      <c r="D31" s="15"/>
-      <c r="E31" s="15"/>
-      <c r="F31" s="15"/>
-      <c r="G31" s="15"/>
-      <c r="H31" s="16"/>
+      <c r="A31" s="9" t="s">
+        <v>53</v>
+      </c>
+      <c r="B31" s="8" t="s">
+        <v>54</v>
+      </c>
+      <c r="C31" s="14"/>
+      <c r="D31" s="23" t="s">
+        <v>29</v>
+      </c>
+      <c r="E31" s="23" t="s">
+        <v>29</v>
+      </c>
+      <c r="F31" s="23"/>
+      <c r="G31" s="14"/>
+      <c r="H31" s="15"/>
       <c r="I31"/>
       <c r="J31"/>
       <c r="K31"/>
@@ -2559,12 +2570,12 @@
     <row r="32" spans="1:43" s="2" customFormat="1" ht="40" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A32" s="9"/>
       <c r="B32" s="8"/>
-      <c r="C32" s="15"/>
-      <c r="D32" s="15"/>
-      <c r="E32" s="15"/>
-      <c r="F32" s="15"/>
-      <c r="G32" s="15"/>
-      <c r="H32" s="16"/>
+      <c r="C32" s="14"/>
+      <c r="D32" s="14"/>
+      <c r="E32" s="14"/>
+      <c r="F32" s="14"/>
+      <c r="G32" s="14"/>
+      <c r="H32" s="15"/>
       <c r="I32"/>
       <c r="J32"/>
       <c r="K32"/>
@@ -2604,12 +2615,12 @@
     <row r="33" spans="1:43" s="2" customFormat="1" ht="40" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A33" s="9"/>
       <c r="B33" s="8"/>
-      <c r="C33" s="15"/>
-      <c r="D33" s="15"/>
-      <c r="E33" s="15"/>
-      <c r="F33" s="15"/>
-      <c r="G33" s="15"/>
-      <c r="H33" s="16"/>
+      <c r="C33" s="14"/>
+      <c r="D33" s="14"/>
+      <c r="E33" s="14"/>
+      <c r="F33" s="14"/>
+      <c r="G33" s="14"/>
+      <c r="H33" s="15"/>
       <c r="I33"/>
       <c r="J33"/>
       <c r="K33"/>
@@ -2649,12 +2660,12 @@
     <row r="34" spans="1:43" s="2" customFormat="1" ht="40" customHeight="1" thickBot="1" x14ac:dyDescent="0.2">
       <c r="A34" s="10"/>
       <c r="B34" s="11"/>
-      <c r="C34" s="17"/>
-      <c r="D34" s="17"/>
-      <c r="E34" s="17"/>
-      <c r="F34" s="17"/>
-      <c r="G34" s="17"/>
-      <c r="H34" s="18"/>
+      <c r="C34" s="16"/>
+      <c r="D34" s="16"/>
+      <c r="E34" s="16"/>
+      <c r="F34" s="16"/>
+      <c r="G34" s="16"/>
+      <c r="H34" s="17"/>
       <c r="I34"/>
       <c r="J34"/>
       <c r="K34"/>
@@ -2784,11 +2795,6 @@
     <row r="81" customFormat="1" x14ac:dyDescent="0.15"/>
   </sheetData>
   <mergeCells count="12">
-    <mergeCell ref="G1:H1"/>
-    <mergeCell ref="A1:F1"/>
-    <mergeCell ref="A3:E3"/>
-    <mergeCell ref="A4:E4"/>
-    <mergeCell ref="F3:H3"/>
     <mergeCell ref="A6:A7"/>
     <mergeCell ref="A2:H2"/>
     <mergeCell ref="A8:H8"/>
@@ -2796,6 +2802,11 @@
     <mergeCell ref="A27:H27"/>
     <mergeCell ref="B6:B7"/>
     <mergeCell ref="A5:H5"/>
+    <mergeCell ref="G1:H1"/>
+    <mergeCell ref="A1:F1"/>
+    <mergeCell ref="A3:E3"/>
+    <mergeCell ref="A4:E4"/>
+    <mergeCell ref="F3:H3"/>
   </mergeCells>
   <phoneticPr fontId="2" type="noConversion"/>
   <printOptions horizontalCentered="1" verticalCentered="1"/>
@@ -2807,14 +2818,12 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement>
-    <lcf76f155ced4ddcb4097134ff3c332f xmlns="44fce352-7b49-42d3-bc69-12da48d9ebc0">
-      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    </lcf76f155ced4ddcb4097134ff3c332f>
-    <TaxCatchAll xmlns="fbb90945-3c4c-43b7-bb15-9ae99079c100" xsi:nil="true"/>
-  </documentManagement>
-</p:properties>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
 </file>
 
 <file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
@@ -3047,27 +3056,20 @@
 </file>
 
 <file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement>
+    <lcf76f155ced4ddcb4097134ff3c332f xmlns="44fce352-7b49-42d3-bc69-12da48d9ebc0">
+      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    </lcf76f155ced4ddcb4097134ff3c332f>
+    <TaxCatchAll xmlns="fbb90945-3c4c-43b7-bb15-9ae99079c100" xsi:nil="true"/>
+  </documentManagement>
+</p:properties>
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{CD1FC233-9ECF-4A55-86D4-136E16072842}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{4209C33D-ED08-404F-9B7A-29CD40C2ACA2}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
-    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
-    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="fbb90945-3c4c-43b7-bb15-9ae99079c100"/>
-    <ds:schemaRef ds:uri="44fce352-7b49-42d3-bc69-12da48d9ebc0"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
@@ -3092,9 +3094,18 @@
 </file>
 
 <file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{4209C33D-ED08-404F-9B7A-29CD40C2ACA2}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{CD1FC233-9ECF-4A55-86D4-136E16072842}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="fbb90945-3c4c-43b7-bb15-9ae99079c100"/>
+    <ds:schemaRef ds:uri="44fce352-7b49-42d3-bc69-12da48d9ebc0"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
</xml_diff>